<commit_message>
Copied in VHDL from HDS after debug of ana_in configurations.
</commit_message>
<xml_diff>
--- a/syscon_usb/DACS_V1_0_ISE/tools/dacs.ucf.xlsx
+++ b/syscon_usb/DACS_V1_0_ISE/tools/dacs.ucf.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="878">
   <si>
     <t>IOSTANDARD</t>
   </si>
@@ -1799,15 +1799,9 @@
     <t>xps_epc_0_PRH_Data_pin&lt;7&gt;</t>
   </si>
   <si>
-    <t>dig_Dir&lt;10&gt;</t>
-  </si>
-  <si>
     <t>ana_in_SCK5&lt;1&gt;</t>
   </si>
   <si>
-    <t>dig_Dir&lt;11&gt;</t>
-  </si>
-  <si>
     <t>subbus_fail_leds&lt;4&gt;</t>
   </si>
   <si>
@@ -1829,9 +1823,6 @@
     <t>xps_epc_0_PRH_Data_pin&lt;5&gt;</t>
   </si>
   <si>
-    <t>dig_Dir&lt;9&gt;</t>
-  </si>
-  <si>
     <t>subbus_fail_leds&lt;2&gt;</t>
   </si>
   <si>
@@ -1880,9 +1871,6 @@
     <t>idx_LimI&lt;0&gt;</t>
   </si>
   <si>
-    <t>dig_Dir&lt;8&gt;</t>
-  </si>
-  <si>
     <t>fpga_0_RS232_RX_pin</t>
   </si>
   <si>
@@ -1913,9 +1901,6 @@
     <t>xps_epc_0_FTDI_RXF_pin</t>
   </si>
   <si>
-    <t>dig_Dir&lt;6&gt;</t>
-  </si>
-  <si>
     <t>dig_IO&lt;3&gt;</t>
   </si>
   <si>
@@ -1937,15 +1922,9 @@
     <t>ana_in_SCK16&lt;0&gt;</t>
   </si>
   <si>
-    <t>dig_Dir&lt;7&gt;</t>
-  </si>
-  <si>
     <t>dig_Dir&lt;2&gt;</t>
   </si>
   <si>
-    <t>dig_Dir&lt;5&gt;</t>
-  </si>
-  <si>
     <t>subbus_fail_leds&lt;0&gt;</t>
   </si>
   <si>
@@ -2021,9 +2000,6 @@
     <t>dig_Dir&lt;1&gt;</t>
   </si>
   <si>
-    <t>dig_Dir&lt;4&gt;</t>
-  </si>
-  <si>
     <t>ana_in_SDI&lt;1&gt;</t>
   </si>
   <si>
@@ -2309,15 +2285,6 @@
     <t>Pulled appropriately</t>
   </si>
   <si>
-    <t>dig_Dir&lt;12&gt;</t>
-  </si>
-  <si>
-    <t>dig_Dir&lt;13&gt;</t>
-  </si>
-  <si>
-    <t>dig_Dir&lt;14&gt;</t>
-  </si>
-  <si>
     <t>DigIO</t>
   </si>
   <si>
@@ -2367,6 +2334,324 @@
   </si>
   <si>
     <t>not subbus_cmdenbl</t>
+  </si>
+  <si>
+    <t>Power Board</t>
+  </si>
+  <si>
+    <t>DigIO/but hard code for input</t>
+  </si>
+  <si>
+    <t>DigIO Input</t>
+  </si>
+  <si>
+    <t>dig_Dir&lt;4&gt;/H</t>
+  </si>
+  <si>
+    <t>dig_Dir&lt;5&gt;/L</t>
+  </si>
+  <si>
+    <t>dig_Dir&lt;6&gt;/L</t>
+  </si>
+  <si>
+    <t>dig_Dir&lt;7&gt;/L</t>
+  </si>
+  <si>
+    <t>dig_Dir&lt;8&gt;/H</t>
+  </si>
+  <si>
+    <t>dig_Dir&lt;9&gt;/H</t>
+  </si>
+  <si>
+    <t>dig_Dir&lt;10&gt;/H</t>
+  </si>
+  <si>
+    <t>dig_Dir&lt;11&gt;/L</t>
+  </si>
+  <si>
+    <t>DigIO Output</t>
+  </si>
+  <si>
+    <t>SW(0)</t>
+  </si>
+  <si>
+    <t>SW(1)</t>
+  </si>
+  <si>
+    <t>SPR_IN(0)</t>
+  </si>
+  <si>
+    <t>SPR_IN(1)</t>
+  </si>
+  <si>
+    <t>CMD(0)</t>
+  </si>
+  <si>
+    <t>CMD(1)</t>
+  </si>
+  <si>
+    <t>CMD(2)</t>
+  </si>
+  <si>
+    <t>CMD(3)</t>
+  </si>
+  <si>
+    <t>CMD(4)</t>
+  </si>
+  <si>
+    <t>CMD(5)</t>
+  </si>
+  <si>
+    <t>CMD(6)</t>
+  </si>
+  <si>
+    <t>CMD(7)</t>
+  </si>
+  <si>
+    <t>CMD(8)</t>
+  </si>
+  <si>
+    <t>CMD(9)</t>
+  </si>
+  <si>
+    <t>CMD(10)</t>
+  </si>
+  <si>
+    <t>CMD(11)</t>
+  </si>
+  <si>
+    <t>CMD(12)</t>
+  </si>
+  <si>
+    <t>CMD(13)</t>
+  </si>
+  <si>
+    <t>CMD(14)</t>
+  </si>
+  <si>
+    <t>CMD(15)</t>
+  </si>
+  <si>
+    <t>CMD(16)</t>
+  </si>
+  <si>
+    <t>CMD(17)</t>
+  </si>
+  <si>
+    <t>CMD(18)</t>
+  </si>
+  <si>
+    <t>CMD(19)</t>
+  </si>
+  <si>
+    <t>CMD(20)</t>
+  </si>
+  <si>
+    <t>CMD(21)</t>
+  </si>
+  <si>
+    <t>CMD(22)</t>
+  </si>
+  <si>
+    <t>CMD(23)</t>
+  </si>
+  <si>
+    <t>CMD_S(1)</t>
+  </si>
+  <si>
+    <t>CMD_S(2)</t>
+  </si>
+  <si>
+    <t>CMD_S(3)</t>
+  </si>
+  <si>
+    <t>CMD_S(4)</t>
+  </si>
+  <si>
+    <t>CMD_S(5)</t>
+  </si>
+  <si>
+    <t>CMD_S(6)</t>
+  </si>
+  <si>
+    <t>CMD_S(7)</t>
+  </si>
+  <si>
+    <t>CMD_S(8)</t>
+  </si>
+  <si>
+    <t>CMD_S(0)</t>
+  </si>
+  <si>
+    <t>CMD_S(9)</t>
+  </si>
+  <si>
+    <t>CMD_S(10)</t>
+  </si>
+  <si>
+    <t>CMD_S(11)</t>
+  </si>
+  <si>
+    <t>CMD_S(12)</t>
+  </si>
+  <si>
+    <t>CMD_S(13)</t>
+  </si>
+  <si>
+    <t>CMD_S(14)</t>
+  </si>
+  <si>
+    <t>CMD_S(15)</t>
+  </si>
+  <si>
+    <t>CMD_S(16)</t>
+  </si>
+  <si>
+    <t>CMD_S(17)</t>
+  </si>
+  <si>
+    <t>CMD_S(18)</t>
+  </si>
+  <si>
+    <t>CMD_S(19)</t>
+  </si>
+  <si>
+    <t>CMD_S(20)</t>
+  </si>
+  <si>
+    <t>CMD_S(21)</t>
+  </si>
+  <si>
+    <t>CMD_S(22)</t>
+  </si>
+  <si>
+    <t>CMD_S(23)</t>
+  </si>
+  <si>
+    <t>CMDI_MUX(0)</t>
+  </si>
+  <si>
+    <t>CMDI_MUX(1)</t>
+  </si>
+  <si>
+    <t>FAIL_LAMP(1)</t>
+  </si>
+  <si>
+    <t>FAIL_LAMP(0)</t>
+  </si>
+  <si>
+    <t>CMDI_MUX(2)</t>
+  </si>
+  <si>
+    <t>PC_RESET</t>
+  </si>
+  <si>
+    <t>CMD Output</t>
+  </si>
+  <si>
+    <t>Cmd&lt;0&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;1&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;2&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;3&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;4&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;5&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;6&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;7&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;8&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;9&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;10&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;11&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;12&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;13&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;14&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;15&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;16&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;17&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;18&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;19&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;20&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;21&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;22&gt;</t>
+  </si>
+  <si>
+    <t>Cmd&lt;23&gt;</t>
+  </si>
+  <si>
+    <t>Pwr_Dir&lt;0&gt;</t>
+  </si>
+  <si>
+    <t>Pwr_Dir&lt;1&gt;</t>
+  </si>
+  <si>
+    <t>Pwr_Dir&lt;2&gt;</t>
+  </si>
+  <si>
+    <t>Pwr_Dir&lt;3&gt;</t>
+  </si>
+  <si>
+    <t>Pwr_Dir&lt;4&gt;</t>
+  </si>
+  <si>
+    <t>Pwr_Dir&lt;5&gt;</t>
+  </si>
+  <si>
+    <t>Pwr_Dir&lt;6&gt;</t>
+  </si>
+  <si>
+    <t>Pwr_Dir&lt;7&gt;</t>
+  </si>
+  <si>
+    <t>ana_in_row&lt;3&gt;</t>
+  </si>
+  <si>
+    <t>ana_in_row&lt;4&gt;</t>
+  </si>
+  <si>
+    <t>ana_in_row&lt;5&gt;</t>
   </si>
 </sst>
 </file>
@@ -2510,7 +2795,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2690,6 +2975,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -2851,7 +3142,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2860,6 +3151,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3198,8 +3490,8 @@
   <dimension ref="A1:K291"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B266" sqref="B266"/>
+      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D179" sqref="D179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3213,18 +3505,19 @@
     <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
     <col min="11" max="11" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
-        <v>755</v>
+        <v>747</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>771</v>
+        <v>760</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>756</v>
+        <v>748</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -3239,7 +3532,7 @@
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>761</v>
+        <v>753</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -3250,7 +3543,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>757</v>
+        <v>749</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
@@ -3270,7 +3563,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>758</v>
+        <v>750</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
@@ -3290,7 +3583,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>669</v>
+        <v>661</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -3307,7 +3600,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
@@ -3324,7 +3617,7 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
@@ -3344,7 +3637,7 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
@@ -3364,7 +3657,7 @@
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>759</v>
+        <v>751</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
@@ -3381,7 +3674,7 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>760</v>
+        <v>752</v>
       </c>
       <c r="E9" t="s">
         <v>5</v>
@@ -3398,7 +3691,7 @@
         <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
@@ -3415,7 +3708,7 @@
         <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
@@ -3432,7 +3725,7 @@
         <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
@@ -3452,7 +3745,7 @@
         <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
@@ -3472,7 +3765,7 @@
         <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>778</v>
+        <v>767</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
@@ -3489,7 +3782,7 @@
         <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>779</v>
+        <v>768</v>
       </c>
       <c r="E15" t="s">
         <v>5</v>
@@ -3506,7 +3799,7 @@
         <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>780</v>
+        <v>769</v>
       </c>
       <c r="E16" t="s">
         <v>5</v>
@@ -3523,7 +3816,7 @@
         <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>778</v>
+        <v>767</v>
       </c>
       <c r="E17" t="s">
         <v>5</v>
@@ -3540,7 +3833,7 @@
         <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>779</v>
+        <v>768</v>
       </c>
       <c r="E18" t="s">
         <v>5</v>
@@ -3557,7 +3850,7 @@
         <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>780</v>
+        <v>769</v>
       </c>
       <c r="E19" t="s">
         <v>5</v>
@@ -4012,7 +4305,7 @@
         <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>646</v>
+        <v>639</v>
       </c>
       <c r="E59" t="s">
         <v>5</v>
@@ -4021,7 +4314,7 @@
         <v>121</v>
       </c>
       <c r="I59" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -4035,7 +4328,7 @@
         <v>1</v>
       </c>
       <c r="D60" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
       <c r="E60" t="s">
         <v>5</v>
@@ -4044,7 +4337,7 @@
         <v>183</v>
       </c>
       <c r="I60" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -4058,7 +4351,7 @@
         <v>2</v>
       </c>
       <c r="D61" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="E61" t="s">
         <v>5</v>
@@ -4067,7 +4360,7 @@
         <v>205</v>
       </c>
       <c r="I61" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -4081,7 +4374,7 @@
         <v>3</v>
       </c>
       <c r="D62" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="E62" t="s">
         <v>5</v>
@@ -4090,7 +4383,7 @@
         <v>227</v>
       </c>
       <c r="I62" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -4104,7 +4397,7 @@
         <v>4</v>
       </c>
       <c r="D63" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="E63" t="s">
         <v>5</v>
@@ -4113,7 +4406,7 @@
         <v>249</v>
       </c>
       <c r="I63" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -4127,7 +4420,7 @@
         <v>5</v>
       </c>
       <c r="D64" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
       <c r="E64" t="s">
         <v>5</v>
@@ -4136,7 +4429,7 @@
         <v>271</v>
       </c>
       <c r="I64" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -4150,7 +4443,7 @@
         <v>6</v>
       </c>
       <c r="D65" t="s">
-        <v>694</v>
+        <v>686</v>
       </c>
       <c r="E65" t="s">
         <v>5</v>
@@ -4159,7 +4452,7 @@
         <v>293</v>
       </c>
       <c r="I65" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -4173,7 +4466,7 @@
         <v>7</v>
       </c>
       <c r="D66" t="s">
-        <v>647</v>
+        <v>640</v>
       </c>
       <c r="E66" t="s">
         <v>5</v>
@@ -4182,7 +4475,7 @@
         <v>315</v>
       </c>
       <c r="I66" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -4196,7 +4489,7 @@
         <v>8</v>
       </c>
       <c r="D67" t="s">
-        <v>648</v>
+        <v>641</v>
       </c>
       <c r="E67" t="s">
         <v>5</v>
@@ -4205,7 +4498,7 @@
         <v>337</v>
       </c>
       <c r="I67" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -4219,7 +4512,7 @@
         <v>9</v>
       </c>
       <c r="D68" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
       <c r="E68" t="s">
         <v>5</v>
@@ -4228,7 +4521,7 @@
         <v>359</v>
       </c>
       <c r="I68" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -4242,7 +4535,7 @@
         <v>10</v>
       </c>
       <c r="D69" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
       <c r="E69" t="s">
         <v>5</v>
@@ -4251,7 +4544,7 @@
         <v>143</v>
       </c>
       <c r="I69" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -4265,7 +4558,7 @@
         <v>11</v>
       </c>
       <c r="D70" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
       <c r="E70" t="s">
         <v>5</v>
@@ -4274,7 +4567,7 @@
         <v>165</v>
       </c>
       <c r="I70" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -4288,7 +4581,7 @@
         <v>12</v>
       </c>
       <c r="D71" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="E71" t="s">
         <v>5</v>
@@ -4297,7 +4590,7 @@
         <v>167</v>
       </c>
       <c r="I71" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -4311,7 +4604,7 @@
         <v>13</v>
       </c>
       <c r="D72" t="s">
-        <v>697</v>
+        <v>689</v>
       </c>
       <c r="E72" t="s">
         <v>5</v>
@@ -4320,7 +4613,7 @@
         <v>169</v>
       </c>
       <c r="I72" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -4334,7 +4627,7 @@
         <v>14</v>
       </c>
       <c r="D73" t="s">
-        <v>696</v>
+        <v>688</v>
       </c>
       <c r="E73" t="s">
         <v>5</v>
@@ -4343,7 +4636,7 @@
         <v>171</v>
       </c>
       <c r="I73" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -4357,7 +4650,7 @@
         <v>15</v>
       </c>
       <c r="D74" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
       <c r="E74" t="s">
         <v>5</v>
@@ -4366,7 +4659,7 @@
         <v>173</v>
       </c>
       <c r="I74" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -4380,7 +4673,7 @@
         <v>16</v>
       </c>
       <c r="D75" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
       <c r="E75" t="s">
         <v>5</v>
@@ -4389,7 +4682,7 @@
         <v>175</v>
       </c>
       <c r="I75" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -4403,7 +4696,7 @@
         <v>17</v>
       </c>
       <c r="D76" t="s">
-        <v>719</v>
+        <v>711</v>
       </c>
       <c r="E76" t="s">
         <v>5</v>
@@ -4412,7 +4705,7 @@
         <v>177</v>
       </c>
       <c r="I76" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -4426,7 +4719,7 @@
         <v>18</v>
       </c>
       <c r="D77" t="s">
-        <v>706</v>
+        <v>698</v>
       </c>
       <c r="E77" t="s">
         <v>5</v>
@@ -4435,7 +4728,7 @@
         <v>179</v>
       </c>
       <c r="I77" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -4449,7 +4742,7 @@
         <v>19</v>
       </c>
       <c r="D78" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
       <c r="E78" t="s">
         <v>5</v>
@@ -4458,7 +4751,7 @@
         <v>181</v>
       </c>
       <c r="I78" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -4472,7 +4765,7 @@
         <v>20</v>
       </c>
       <c r="D79" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
       <c r="E79" t="s">
         <v>5</v>
@@ -4481,7 +4774,7 @@
         <v>185</v>
       </c>
       <c r="I79" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -4495,7 +4788,7 @@
         <v>21</v>
       </c>
       <c r="D80" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
       <c r="E80" t="s">
         <v>5</v>
@@ -4504,7 +4797,7 @@
         <v>187</v>
       </c>
       <c r="I80" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -4518,7 +4811,7 @@
         <v>22</v>
       </c>
       <c r="D81" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
       <c r="E81" t="s">
         <v>5</v>
@@ -4527,7 +4820,7 @@
         <v>189</v>
       </c>
       <c r="I81" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -4541,7 +4834,7 @@
         <v>23</v>
       </c>
       <c r="D82" t="s">
-        <v>707</v>
+        <v>699</v>
       </c>
       <c r="E82" t="s">
         <v>5</v>
@@ -4550,7 +4843,7 @@
         <v>191</v>
       </c>
       <c r="I82" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -4564,7 +4857,7 @@
         <v>24</v>
       </c>
       <c r="D83" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="E83" t="s">
         <v>5</v>
@@ -4573,7 +4866,7 @@
         <v>193</v>
       </c>
       <c r="I83" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -4587,7 +4880,7 @@
         <v>25</v>
       </c>
       <c r="D84" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E84" t="s">
         <v>5</v>
@@ -4596,7 +4889,7 @@
         <v>195</v>
       </c>
       <c r="I84" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -4610,7 +4903,7 @@
         <v>26</v>
       </c>
       <c r="D85" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
       <c r="E85" t="s">
         <v>5</v>
@@ -4619,7 +4912,7 @@
         <v>197</v>
       </c>
       <c r="I85" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -4633,7 +4926,7 @@
         <v>27</v>
       </c>
       <c r="D86" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="E86" t="s">
         <v>5</v>
@@ -4642,7 +4935,7 @@
         <v>199</v>
       </c>
       <c r="I86" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -4656,7 +4949,7 @@
         <v>28</v>
       </c>
       <c r="D87" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="E87" t="s">
         <v>5</v>
@@ -4665,7 +4958,7 @@
         <v>201</v>
       </c>
       <c r="I87" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -4679,7 +4972,7 @@
         <v>29</v>
       </c>
       <c r="D88" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="E88" t="s">
         <v>5</v>
@@ -4688,7 +4981,7 @@
         <v>203</v>
       </c>
       <c r="I88" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -4702,7 +4995,7 @@
         <v>30</v>
       </c>
       <c r="D89" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
       <c r="E89" t="s">
         <v>5</v>
@@ -4711,7 +5004,7 @@
         <v>207</v>
       </c>
       <c r="I89" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -4725,7 +5018,7 @@
         <v>31</v>
       </c>
       <c r="D90" t="s">
-        <v>653</v>
+        <v>646</v>
       </c>
       <c r="E90" t="s">
         <v>5</v>
@@ -4734,7 +5027,7 @@
         <v>209</v>
       </c>
       <c r="I90" t="s">
-        <v>767</v>
+        <v>756</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -4748,7 +5041,7 @@
         <v>32</v>
       </c>
       <c r="D91" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="E91" t="s">
         <v>5</v>
@@ -4757,7 +5050,7 @@
         <v>211</v>
       </c>
       <c r="I91" t="s">
-        <v>768</v>
+        <v>757</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -4777,7 +5070,7 @@
         <v>213</v>
       </c>
       <c r="I92" t="s">
-        <v>768</v>
+        <v>757</v>
       </c>
     </row>
     <row r="93" spans="1:9">
@@ -4797,7 +5090,7 @@
         <v>215</v>
       </c>
       <c r="I93" t="s">
-        <v>768</v>
+        <v>757</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -4817,7 +5110,7 @@
         <v>217</v>
       </c>
       <c r="I94" t="s">
-        <v>768</v>
+        <v>757</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -4837,7 +5130,7 @@
         <v>219</v>
       </c>
       <c r="I95" t="s">
-        <v>768</v>
+        <v>757</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -4857,7 +5150,7 @@
         <v>221</v>
       </c>
       <c r="I96" t="s">
-        <v>768</v>
+        <v>757</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -4877,7 +5170,7 @@
         <v>223</v>
       </c>
       <c r="I97" t="s">
-        <v>768</v>
+        <v>757</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -4897,7 +5190,7 @@
         <v>225</v>
       </c>
       <c r="I98" t="s">
-        <v>768</v>
+        <v>757</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -4911,7 +5204,7 @@
         <v>40</v>
       </c>
       <c r="D99" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="E99" t="s">
         <v>5</v>
@@ -4920,7 +5213,7 @@
         <v>229</v>
       </c>
       <c r="I99" t="s">
-        <v>769</v>
+        <v>758</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -4934,7 +5227,7 @@
         <v>41</v>
       </c>
       <c r="D100" t="s">
-        <v>644</v>
+        <v>637</v>
       </c>
       <c r="E100" t="s">
         <v>5</v>
@@ -4943,7 +5236,7 @@
         <v>231</v>
       </c>
       <c r="I100" t="s">
-        <v>769</v>
+        <v>758</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -4957,7 +5250,7 @@
         <v>42</v>
       </c>
       <c r="D101" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="E101" t="s">
         <v>5</v>
@@ -4966,7 +5259,7 @@
         <v>233</v>
       </c>
       <c r="I101" t="s">
-        <v>769</v>
+        <v>758</v>
       </c>
     </row>
     <row r="102" spans="1:9">
@@ -4980,7 +5273,7 @@
         <v>43</v>
       </c>
       <c r="D102" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="E102" t="s">
         <v>5</v>
@@ -4989,7 +5282,7 @@
         <v>235</v>
       </c>
       <c r="I102" t="s">
-        <v>769</v>
+        <v>758</v>
       </c>
     </row>
     <row r="103" spans="1:9">
@@ -5003,7 +5296,7 @@
         <v>44</v>
       </c>
       <c r="D103" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="E103" t="s">
         <v>5</v>
@@ -5012,7 +5305,7 @@
         <v>237</v>
       </c>
       <c r="I103" t="s">
-        <v>769</v>
+        <v>758</v>
       </c>
     </row>
     <row r="104" spans="1:9">
@@ -5026,7 +5319,7 @@
         <v>45</v>
       </c>
       <c r="D104" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E104" t="s">
         <v>5</v>
@@ -5035,7 +5328,7 @@
         <v>239</v>
       </c>
       <c r="I104" t="s">
-        <v>769</v>
+        <v>758</v>
       </c>
     </row>
     <row r="105" spans="1:9">
@@ -5049,7 +5342,7 @@
         <v>46</v>
       </c>
       <c r="D105" t="s">
-        <v>645</v>
+        <v>638</v>
       </c>
       <c r="E105" t="s">
         <v>5</v>
@@ -5058,7 +5351,7 @@
         <v>241</v>
       </c>
       <c r="I105" t="s">
-        <v>769</v>
+        <v>758</v>
       </c>
     </row>
     <row r="106" spans="1:9">
@@ -5072,7 +5365,7 @@
         <v>47</v>
       </c>
       <c r="D106" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="E106" t="s">
         <v>5</v>
@@ -5081,7 +5374,7 @@
         <v>243</v>
       </c>
       <c r="I106" t="s">
-        <v>769</v>
+        <v>758</v>
       </c>
     </row>
     <row r="107" spans="1:9">
@@ -5095,7 +5388,7 @@
         <v>48</v>
       </c>
       <c r="D107" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="E107" t="s">
         <v>5</v>
@@ -5104,7 +5397,7 @@
         <v>245</v>
       </c>
       <c r="I107" t="s">
-        <v>769</v>
+        <v>758</v>
       </c>
     </row>
     <row r="108" spans="1:9">
@@ -5118,7 +5411,7 @@
         <v>49</v>
       </c>
       <c r="D108" t="s">
-        <v>691</v>
+        <v>683</v>
       </c>
       <c r="E108" t="s">
         <v>5</v>
@@ -5127,7 +5420,7 @@
         <v>247</v>
       </c>
       <c r="I108" t="s">
-        <v>769</v>
+        <v>758</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -5141,7 +5434,7 @@
         <v>50</v>
       </c>
       <c r="D109" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="E109" t="s">
         <v>5</v>
@@ -5150,7 +5443,7 @@
         <v>251</v>
       </c>
       <c r="I109" t="s">
-        <v>769</v>
+        <v>758</v>
       </c>
     </row>
     <row r="110" spans="1:9">
@@ -5164,7 +5457,7 @@
         <v>51</v>
       </c>
       <c r="D110" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="E110" t="s">
         <v>5</v>
@@ -5173,7 +5466,7 @@
         <v>253</v>
       </c>
       <c r="I110" t="s">
-        <v>769</v>
+        <v>758</v>
       </c>
     </row>
     <row r="111" spans="1:9">
@@ -5187,7 +5480,7 @@
         <v>52</v>
       </c>
       <c r="D111" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
       <c r="E111" t="s">
         <v>5</v>
@@ -5196,7 +5489,7 @@
         <v>255</v>
       </c>
       <c r="I111" t="s">
-        <v>769</v>
+        <v>758</v>
       </c>
     </row>
     <row r="112" spans="1:9">
@@ -5210,7 +5503,7 @@
         <v>53</v>
       </c>
       <c r="D112" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="E112" t="s">
         <v>5</v>
@@ -5219,10 +5512,10 @@
         <v>257</v>
       </c>
       <c r="I112" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11">
       <c r="A113">
         <v>1</v>
       </c>
@@ -5233,7 +5526,7 @@
         <v>54</v>
       </c>
       <c r="D113" t="s">
-        <v>692</v>
+        <v>684</v>
       </c>
       <c r="E113" t="s">
         <v>5</v>
@@ -5242,10 +5535,10 @@
         <v>259</v>
       </c>
       <c r="I113" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11">
       <c r="B114" t="s">
         <v>260</v>
       </c>
@@ -5259,10 +5552,10 @@
         <v>261</v>
       </c>
       <c r="I114" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11">
       <c r="A115">
         <v>1</v>
       </c>
@@ -5273,7 +5566,7 @@
         <v>56</v>
       </c>
       <c r="D115" t="s">
-        <v>740</v>
+        <v>732</v>
       </c>
       <c r="E115" t="s">
         <v>5</v>
@@ -5282,10 +5575,10 @@
         <v>263</v>
       </c>
       <c r="I115" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11">
       <c r="A116">
         <v>1</v>
       </c>
@@ -5296,7 +5589,7 @@
         <v>57</v>
       </c>
       <c r="D116" t="s">
-        <v>743</v>
+        <v>735</v>
       </c>
       <c r="E116" t="s">
         <v>5</v>
@@ -5305,10 +5598,10 @@
         <v>265</v>
       </c>
       <c r="I116" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11">
       <c r="A117">
         <v>1</v>
       </c>
@@ -5319,7 +5612,7 @@
         <v>58</v>
       </c>
       <c r="D117" t="s">
-        <v>744</v>
+        <v>736</v>
       </c>
       <c r="E117" t="s">
         <v>5</v>
@@ -5328,10 +5621,10 @@
         <v>267</v>
       </c>
       <c r="I117" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11">
       <c r="A118">
         <v>1</v>
       </c>
@@ -5342,7 +5635,7 @@
         <v>59</v>
       </c>
       <c r="D118" t="s">
-        <v>747</v>
+        <v>739</v>
       </c>
       <c r="E118" t="s">
         <v>5</v>
@@ -5351,10 +5644,10 @@
         <v>269</v>
       </c>
       <c r="I118" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11">
       <c r="A119">
         <v>1</v>
       </c>
@@ -5365,7 +5658,7 @@
         <v>60</v>
       </c>
       <c r="D119" t="s">
-        <v>717</v>
+        <v>709</v>
       </c>
       <c r="E119" t="s">
         <v>5</v>
@@ -5374,10 +5667,16 @@
         <v>273</v>
       </c>
       <c r="I119" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J119" t="s">
+        <v>772</v>
+      </c>
+      <c r="K119" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11">
       <c r="A120">
         <v>1</v>
       </c>
@@ -5388,7 +5687,7 @@
         <v>61</v>
       </c>
       <c r="D120" t="s">
-        <v>704</v>
+        <v>696</v>
       </c>
       <c r="E120" t="s">
         <v>5</v>
@@ -5397,10 +5696,16 @@
         <v>275</v>
       </c>
       <c r="I120" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J120" t="s">
+        <v>772</v>
+      </c>
+      <c r="K120" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11">
       <c r="A121">
         <v>1</v>
       </c>
@@ -5411,7 +5716,7 @@
         <v>62</v>
       </c>
       <c r="D121" t="s">
-        <v>748</v>
+        <v>740</v>
       </c>
       <c r="E121" t="s">
         <v>5</v>
@@ -5420,10 +5725,16 @@
         <v>277</v>
       </c>
       <c r="I121" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J121" t="s">
+        <v>772</v>
+      </c>
+      <c r="K121" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11">
       <c r="A122">
         <v>1</v>
       </c>
@@ -5434,7 +5745,7 @@
         <v>63</v>
       </c>
       <c r="D122" t="s">
-        <v>718</v>
+        <v>710</v>
       </c>
       <c r="E122" t="s">
         <v>5</v>
@@ -5443,10 +5754,16 @@
         <v>279</v>
       </c>
       <c r="I122" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J122" t="s">
+        <v>772</v>
+      </c>
+      <c r="K122" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11">
       <c r="A123">
         <v>1</v>
       </c>
@@ -5457,7 +5774,7 @@
         <v>64</v>
       </c>
       <c r="D123" t="s">
-        <v>751</v>
+        <v>843</v>
       </c>
       <c r="E123" t="s">
         <v>5</v>
@@ -5466,10 +5783,16 @@
         <v>281</v>
       </c>
       <c r="I123" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J123" t="s">
+        <v>772</v>
+      </c>
+      <c r="K123" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11">
       <c r="A124">
         <v>1</v>
       </c>
@@ -5480,7 +5803,7 @@
         <v>65</v>
       </c>
       <c r="D124" t="s">
-        <v>752</v>
+        <v>844</v>
       </c>
       <c r="E124" t="s">
         <v>5</v>
@@ -5489,10 +5812,16 @@
         <v>283</v>
       </c>
       <c r="I124" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J124" t="s">
+        <v>772</v>
+      </c>
+      <c r="K124" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11">
       <c r="A125">
         <v>1</v>
       </c>
@@ -5503,7 +5832,7 @@
         <v>66</v>
       </c>
       <c r="D125" t="s">
-        <v>725</v>
+        <v>845</v>
       </c>
       <c r="E125" t="s">
         <v>5</v>
@@ -5512,10 +5841,16 @@
         <v>285</v>
       </c>
       <c r="I125" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J125" t="s">
+        <v>772</v>
+      </c>
+      <c r="K125" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11">
       <c r="A126">
         <v>1</v>
       </c>
@@ -5526,7 +5861,7 @@
         <v>67</v>
       </c>
       <c r="D126" t="s">
-        <v>732</v>
+        <v>846</v>
       </c>
       <c r="E126" t="s">
         <v>5</v>
@@ -5535,10 +5870,16 @@
         <v>287</v>
       </c>
       <c r="I126" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J126" t="s">
+        <v>772</v>
+      </c>
+      <c r="K126" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11">
       <c r="A127">
         <v>1</v>
       </c>
@@ -5549,7 +5890,7 @@
         <v>68</v>
       </c>
       <c r="D127" t="s">
-        <v>733</v>
+        <v>847</v>
       </c>
       <c r="E127" t="s">
         <v>5</v>
@@ -5558,10 +5899,16 @@
         <v>289</v>
       </c>
       <c r="I127" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J127" t="s">
+        <v>772</v>
+      </c>
+      <c r="K127" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11">
       <c r="A128">
         <v>1</v>
       </c>
@@ -5572,7 +5919,7 @@
         <v>69</v>
       </c>
       <c r="D128" t="s">
-        <v>753</v>
+        <v>848</v>
       </c>
       <c r="E128" t="s">
         <v>5</v>
@@ -5581,10 +5928,16 @@
         <v>291</v>
       </c>
       <c r="I128" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J128" t="s">
+        <v>772</v>
+      </c>
+      <c r="K128" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11">
       <c r="A129">
         <v>1</v>
       </c>
@@ -5595,7 +5948,7 @@
         <v>70</v>
       </c>
       <c r="D129" t="s">
-        <v>754</v>
+        <v>849</v>
       </c>
       <c r="E129" t="s">
         <v>5</v>
@@ -5604,10 +5957,16 @@
         <v>295</v>
       </c>
       <c r="I129" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J129" t="s">
+        <v>772</v>
+      </c>
+      <c r="K129" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11">
       <c r="A130">
         <v>1</v>
       </c>
@@ -5618,7 +5977,7 @@
         <v>71</v>
       </c>
       <c r="D130" t="s">
-        <v>705</v>
+        <v>850</v>
       </c>
       <c r="E130" t="s">
         <v>5</v>
@@ -5627,10 +5986,16 @@
         <v>297</v>
       </c>
       <c r="I130" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J130" t="s">
+        <v>772</v>
+      </c>
+      <c r="K130" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11">
       <c r="A131">
         <v>1</v>
       </c>
@@ -5641,7 +6006,7 @@
         <v>72</v>
       </c>
       <c r="D131" t="s">
-        <v>695</v>
+        <v>851</v>
       </c>
       <c r="E131" t="s">
         <v>5</v>
@@ -5650,10 +6015,16 @@
         <v>299</v>
       </c>
       <c r="I131" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J131" t="s">
+        <v>772</v>
+      </c>
+      <c r="K131" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11">
       <c r="A132">
         <v>1</v>
       </c>
@@ -5664,7 +6035,7 @@
         <v>73</v>
       </c>
       <c r="D132" t="s">
-        <v>715</v>
+        <v>852</v>
       </c>
       <c r="E132" t="s">
         <v>5</v>
@@ -5673,10 +6044,16 @@
         <v>301</v>
       </c>
       <c r="I132" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J132" t="s">
+        <v>772</v>
+      </c>
+      <c r="K132" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11">
       <c r="A133">
         <v>1</v>
       </c>
@@ -5687,7 +6064,7 @@
         <v>74</v>
       </c>
       <c r="D133" t="s">
-        <v>716</v>
+        <v>853</v>
       </c>
       <c r="E133" t="s">
         <v>5</v>
@@ -5696,10 +6073,16 @@
         <v>303</v>
       </c>
       <c r="I133" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J133" t="s">
+        <v>772</v>
+      </c>
+      <c r="K133" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11">
       <c r="A134">
         <v>1</v>
       </c>
@@ -5710,7 +6093,7 @@
         <v>75</v>
       </c>
       <c r="D134" t="s">
-        <v>746</v>
+        <v>854</v>
       </c>
       <c r="E134" t="s">
         <v>5</v>
@@ -5719,10 +6102,16 @@
         <v>305</v>
       </c>
       <c r="I134" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J134" t="s">
+        <v>772</v>
+      </c>
+      <c r="K134" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11">
       <c r="A135">
         <v>1</v>
       </c>
@@ -5733,7 +6122,7 @@
         <v>76</v>
       </c>
       <c r="D135" t="s">
-        <v>731</v>
+        <v>855</v>
       </c>
       <c r="E135" t="s">
         <v>5</v>
@@ -5742,10 +6131,16 @@
         <v>307</v>
       </c>
       <c r="I135" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J135" t="s">
+        <v>772</v>
+      </c>
+      <c r="K135" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11">
       <c r="A136">
         <v>1</v>
       </c>
@@ -5756,7 +6151,7 @@
         <v>77</v>
       </c>
       <c r="D136" t="s">
-        <v>738</v>
+        <v>856</v>
       </c>
       <c r="E136" t="s">
         <v>5</v>
@@ -5765,10 +6160,16 @@
         <v>309</v>
       </c>
       <c r="I136" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J136" t="s">
+        <v>772</v>
+      </c>
+      <c r="K136" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11">
       <c r="A137">
         <v>1</v>
       </c>
@@ -5779,7 +6180,7 @@
         <v>78</v>
       </c>
       <c r="D137" t="s">
-        <v>703</v>
+        <v>857</v>
       </c>
       <c r="E137" t="s">
         <v>5</v>
@@ -5788,10 +6189,16 @@
         <v>311</v>
       </c>
       <c r="I137" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J137" t="s">
+        <v>772</v>
+      </c>
+      <c r="K137" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11">
       <c r="A138">
         <v>1</v>
       </c>
@@ -5802,7 +6209,7 @@
         <v>79</v>
       </c>
       <c r="D138" t="s">
-        <v>745</v>
+        <v>858</v>
       </c>
       <c r="E138" t="s">
         <v>5</v>
@@ -5811,10 +6218,16 @@
         <v>313</v>
       </c>
       <c r="I138" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J138" t="s">
+        <v>772</v>
+      </c>
+      <c r="K138" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11">
       <c r="A139">
         <v>1</v>
       </c>
@@ -5825,7 +6238,7 @@
         <v>80</v>
       </c>
       <c r="D139" t="s">
-        <v>750</v>
+        <v>859</v>
       </c>
       <c r="E139" t="s">
         <v>5</v>
@@ -5834,10 +6247,16 @@
         <v>317</v>
       </c>
       <c r="I139" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J139" t="s">
+        <v>772</v>
+      </c>
+      <c r="K139" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11">
       <c r="A140">
         <v>1</v>
       </c>
@@ -5848,7 +6267,7 @@
         <v>81</v>
       </c>
       <c r="D140" t="s">
-        <v>713</v>
+        <v>860</v>
       </c>
       <c r="E140" t="s">
         <v>5</v>
@@ -5857,10 +6276,16 @@
         <v>319</v>
       </c>
       <c r="I140" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J140" t="s">
+        <v>772</v>
+      </c>
+      <c r="K140" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11">
       <c r="A141">
         <v>1</v>
       </c>
@@ -5871,7 +6296,7 @@
         <v>82</v>
       </c>
       <c r="D141" t="s">
-        <v>714</v>
+        <v>861</v>
       </c>
       <c r="E141" t="s">
         <v>5</v>
@@ -5880,10 +6305,16 @@
         <v>321</v>
       </c>
       <c r="I141" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J141" t="s">
+        <v>772</v>
+      </c>
+      <c r="K141" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11">
       <c r="A142">
         <v>1</v>
       </c>
@@ -5894,7 +6325,7 @@
         <v>83</v>
       </c>
       <c r="D142" t="s">
-        <v>724</v>
+        <v>862</v>
       </c>
       <c r="E142" t="s">
         <v>5</v>
@@ -5903,10 +6334,16 @@
         <v>323</v>
       </c>
       <c r="I142" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J142" t="s">
+        <v>772</v>
+      </c>
+      <c r="K142" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11">
       <c r="A143">
         <v>1</v>
       </c>
@@ -5917,7 +6354,7 @@
         <v>84</v>
       </c>
       <c r="D143" t="s">
-        <v>741</v>
+        <v>863</v>
       </c>
       <c r="E143" t="s">
         <v>5</v>
@@ -5926,10 +6363,16 @@
         <v>325</v>
       </c>
       <c r="I143" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="144" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J143" t="s">
+        <v>772</v>
+      </c>
+      <c r="K143" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11">
       <c r="A144">
         <v>1</v>
       </c>
@@ -5940,7 +6383,7 @@
         <v>85</v>
       </c>
       <c r="D144" t="s">
-        <v>712</v>
+        <v>864</v>
       </c>
       <c r="E144" t="s">
         <v>5</v>
@@ -5949,10 +6392,16 @@
         <v>327</v>
       </c>
       <c r="I144" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J144" t="s">
+        <v>772</v>
+      </c>
+      <c r="K144" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11">
       <c r="A145">
         <v>1</v>
       </c>
@@ -5963,7 +6412,7 @@
         <v>86</v>
       </c>
       <c r="D145" t="s">
-        <v>730</v>
+        <v>865</v>
       </c>
       <c r="E145" t="s">
         <v>5</v>
@@ -5972,10 +6421,16 @@
         <v>329</v>
       </c>
       <c r="I145" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="146" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J145" t="s">
+        <v>772</v>
+      </c>
+      <c r="K145" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11">
       <c r="A146">
         <v>1</v>
       </c>
@@ -5986,7 +6441,7 @@
         <v>87</v>
       </c>
       <c r="D146" t="s">
-        <v>742</v>
+        <v>866</v>
       </c>
       <c r="E146" t="s">
         <v>5</v>
@@ -5995,10 +6450,16 @@
         <v>331</v>
       </c>
       <c r="I146" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="147" spans="1:9">
+        <v>842</v>
+      </c>
+      <c r="J146" t="s">
+        <v>772</v>
+      </c>
+      <c r="K146" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11">
       <c r="A147">
         <v>1</v>
       </c>
@@ -6009,7 +6470,7 @@
         <v>88</v>
       </c>
       <c r="D147" t="s">
-        <v>749</v>
+        <v>741</v>
       </c>
       <c r="E147" t="s">
         <v>5</v>
@@ -6018,10 +6479,16 @@
         <v>333</v>
       </c>
       <c r="I147" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="148" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J147" t="s">
+        <v>772</v>
+      </c>
+      <c r="K147" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11">
       <c r="A148">
         <v>1</v>
       </c>
@@ -6032,7 +6499,7 @@
         <v>89</v>
       </c>
       <c r="D148" t="s">
-        <v>737</v>
+        <v>729</v>
       </c>
       <c r="E148" t="s">
         <v>5</v>
@@ -6041,10 +6508,16 @@
         <v>335</v>
       </c>
       <c r="I148" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="149" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J148" t="s">
+        <v>772</v>
+      </c>
+      <c r="K148" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11">
       <c r="A149">
         <v>1</v>
       </c>
@@ -6055,7 +6528,7 @@
         <v>90</v>
       </c>
       <c r="D149" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="E149" t="s">
         <v>5</v>
@@ -6064,10 +6537,16 @@
         <v>339</v>
       </c>
       <c r="I149" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="150" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J149" t="s">
+        <v>772</v>
+      </c>
+      <c r="K149" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11">
       <c r="A150">
         <v>1</v>
       </c>
@@ -6078,7 +6557,7 @@
         <v>91</v>
       </c>
       <c r="D150" t="s">
-        <v>729</v>
+        <v>721</v>
       </c>
       <c r="E150" t="s">
         <v>5</v>
@@ -6087,10 +6566,16 @@
         <v>341</v>
       </c>
       <c r="I150" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="151" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J150" t="s">
+        <v>772</v>
+      </c>
+      <c r="K150" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11">
       <c r="A151">
         <v>1</v>
       </c>
@@ -6101,7 +6586,7 @@
         <v>92</v>
       </c>
       <c r="D151" t="s">
-        <v>728</v>
+        <v>720</v>
       </c>
       <c r="E151" t="s">
         <v>5</v>
@@ -6110,10 +6595,16 @@
         <v>343</v>
       </c>
       <c r="I151" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="152" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J151" t="s">
+        <v>772</v>
+      </c>
+      <c r="K151" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11">
       <c r="A152">
         <v>1</v>
       </c>
@@ -6124,7 +6615,7 @@
         <v>93</v>
       </c>
       <c r="D152" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
       <c r="E152" t="s">
         <v>5</v>
@@ -6133,10 +6624,16 @@
         <v>345</v>
       </c>
       <c r="I152" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="153" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J152" t="s">
+        <v>772</v>
+      </c>
+      <c r="K152" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11">
       <c r="A153">
         <v>1</v>
       </c>
@@ -6147,7 +6644,7 @@
         <v>94</v>
       </c>
       <c r="D153" t="s">
-        <v>722</v>
+        <v>714</v>
       </c>
       <c r="E153" t="s">
         <v>5</v>
@@ -6156,10 +6653,16 @@
         <v>347</v>
       </c>
       <c r="I153" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="154" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J153" t="s">
+        <v>772</v>
+      </c>
+      <c r="K153" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11">
       <c r="A154">
         <v>1</v>
       </c>
@@ -6170,7 +6673,7 @@
         <v>95</v>
       </c>
       <c r="D154" t="s">
-        <v>710</v>
+        <v>702</v>
       </c>
       <c r="E154" t="s">
         <v>5</v>
@@ -6179,10 +6682,16 @@
         <v>349</v>
       </c>
       <c r="I154" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="155" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J154" t="s">
+        <v>772</v>
+      </c>
+      <c r="K154" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11">
       <c r="A155">
         <v>1</v>
       </c>
@@ -6193,7 +6702,7 @@
         <v>96</v>
       </c>
       <c r="D155" t="s">
-        <v>709</v>
+        <v>701</v>
       </c>
       <c r="E155" t="s">
         <v>5</v>
@@ -6202,10 +6711,16 @@
         <v>351</v>
       </c>
       <c r="I155" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="156" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J155" t="s">
+        <v>772</v>
+      </c>
+      <c r="K155" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11">
       <c r="A156">
         <v>1</v>
       </c>
@@ -6216,7 +6731,7 @@
         <v>97</v>
       </c>
       <c r="D156" t="s">
-        <v>701</v>
+        <v>693</v>
       </c>
       <c r="E156" t="s">
         <v>5</v>
@@ -6225,10 +6740,16 @@
         <v>353</v>
       </c>
       <c r="I156" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="157" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J156" t="s">
+        <v>772</v>
+      </c>
+      <c r="K156" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11">
       <c r="A157">
         <v>1</v>
       </c>
@@ -6239,7 +6760,7 @@
         <v>98</v>
       </c>
       <c r="D157" t="s">
-        <v>700</v>
+        <v>692</v>
       </c>
       <c r="E157" t="s">
         <v>5</v>
@@ -6248,10 +6769,16 @@
         <v>355</v>
       </c>
       <c r="I157" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="158" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J157" t="s">
+        <v>772</v>
+      </c>
+      <c r="K157" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11">
       <c r="A158">
         <v>1</v>
       </c>
@@ -6262,7 +6789,7 @@
         <v>99</v>
       </c>
       <c r="D158" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
       <c r="E158" t="s">
         <v>5</v>
@@ -6271,10 +6798,16 @@
         <v>357</v>
       </c>
       <c r="I158" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="159" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J158" t="s">
+        <v>772</v>
+      </c>
+      <c r="K158" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11">
       <c r="A159">
         <v>1</v>
       </c>
@@ -6285,7 +6818,7 @@
         <v>100</v>
       </c>
       <c r="D159" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
       <c r="E159" t="s">
         <v>5</v>
@@ -6294,10 +6827,16 @@
         <v>123</v>
       </c>
       <c r="I159" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="160" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J159" t="s">
+        <v>772</v>
+      </c>
+      <c r="K159" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11">
       <c r="A160">
         <v>1</v>
       </c>
@@ -6308,7 +6847,7 @@
         <v>101</v>
       </c>
       <c r="D160" t="s">
-        <v>676</v>
+        <v>668</v>
       </c>
       <c r="E160" t="s">
         <v>5</v>
@@ -6317,10 +6856,16 @@
         <v>125</v>
       </c>
       <c r="I160" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="161" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J160" t="s">
+        <v>772</v>
+      </c>
+      <c r="K160" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11">
       <c r="A161">
         <v>1</v>
       </c>
@@ -6331,7 +6876,7 @@
         <v>102</v>
       </c>
       <c r="D161" t="s">
-        <v>675</v>
+        <v>667</v>
       </c>
       <c r="E161" t="s">
         <v>5</v>
@@ -6340,10 +6885,16 @@
         <v>127</v>
       </c>
       <c r="I161" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="162" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J161" t="s">
+        <v>772</v>
+      </c>
+      <c r="K161" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11">
       <c r="A162">
         <v>1</v>
       </c>
@@ -6354,7 +6905,7 @@
         <v>103</v>
       </c>
       <c r="D162" t="s">
-        <v>711</v>
+        <v>703</v>
       </c>
       <c r="E162" t="s">
         <v>5</v>
@@ -6363,10 +6914,16 @@
         <v>129</v>
       </c>
       <c r="I162" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="163" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J162" t="s">
+        <v>772</v>
+      </c>
+      <c r="K162" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11">
       <c r="A163">
         <v>1</v>
       </c>
@@ -6377,7 +6934,7 @@
         <v>104</v>
       </c>
       <c r="D163" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="E163" t="s">
         <v>5</v>
@@ -6386,10 +6943,16 @@
         <v>131</v>
       </c>
       <c r="I163" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="164" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J163" t="s">
+        <v>772</v>
+      </c>
+      <c r="K163" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11">
       <c r="A164">
         <v>1</v>
       </c>
@@ -6400,7 +6963,7 @@
         <v>105</v>
       </c>
       <c r="D164" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="E164" t="s">
         <v>5</v>
@@ -6409,10 +6972,16 @@
         <v>133</v>
       </c>
       <c r="I164" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="165" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J164" t="s">
+        <v>772</v>
+      </c>
+      <c r="K164" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11">
       <c r="A165">
         <v>1</v>
       </c>
@@ -6423,7 +6992,7 @@
         <v>106</v>
       </c>
       <c r="D165" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="E165" t="s">
         <v>5</v>
@@ -6432,10 +7001,16 @@
         <v>135</v>
       </c>
       <c r="I165" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="166" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J165" t="s">
+        <v>772</v>
+      </c>
+      <c r="K165" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11">
       <c r="A166">
         <v>1</v>
       </c>
@@ -6446,7 +7021,7 @@
         <v>107</v>
       </c>
       <c r="D166" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
       <c r="E166" t="s">
         <v>5</v>
@@ -6455,10 +7030,16 @@
         <v>137</v>
       </c>
       <c r="I166" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="167" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J166" t="s">
+        <v>772</v>
+      </c>
+      <c r="K166" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11">
       <c r="A167">
         <v>1</v>
       </c>
@@ -6469,7 +7050,7 @@
         <v>108</v>
       </c>
       <c r="D167" t="s">
-        <v>690</v>
+        <v>682</v>
       </c>
       <c r="E167" t="s">
         <v>5</v>
@@ -6478,10 +7059,16 @@
         <v>139</v>
       </c>
       <c r="I167" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J167" t="s">
+        <v>772</v>
+      </c>
+      <c r="K167" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11">
       <c r="A168">
         <v>1</v>
       </c>
@@ -6492,7 +7079,7 @@
         <v>109</v>
       </c>
       <c r="D168" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
       <c r="E168" t="s">
         <v>5</v>
@@ -6501,10 +7088,16 @@
         <v>141</v>
       </c>
       <c r="I168" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="169" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J168" t="s">
+        <v>772</v>
+      </c>
+      <c r="K168" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11">
       <c r="A169">
         <v>1</v>
       </c>
@@ -6515,7 +7108,7 @@
         <v>110</v>
       </c>
       <c r="D169" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
       <c r="E169" t="s">
         <v>5</v>
@@ -6524,10 +7117,16 @@
         <v>145</v>
       </c>
       <c r="I169" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="170" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J169" t="s">
+        <v>772</v>
+      </c>
+      <c r="K169" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11">
       <c r="A170">
         <v>1</v>
       </c>
@@ -6538,7 +7137,7 @@
         <v>111</v>
       </c>
       <c r="D170" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="E170" t="s">
         <v>5</v>
@@ -6547,10 +7146,16 @@
         <v>147</v>
       </c>
       <c r="I170" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="171" spans="1:9">
+        <v>774</v>
+      </c>
+      <c r="J170" t="s">
+        <v>772</v>
+      </c>
+      <c r="K170" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11">
       <c r="A171">
         <v>1</v>
       </c>
@@ -6561,7 +7166,7 @@
         <v>112</v>
       </c>
       <c r="D171" t="s">
-        <v>661</v>
+        <v>875</v>
       </c>
       <c r="E171" t="s">
         <v>5</v>
@@ -6570,10 +7175,16 @@
         <v>149</v>
       </c>
       <c r="I171" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="172" spans="1:9">
+        <v>783</v>
+      </c>
+      <c r="J171" t="s">
+        <v>772</v>
+      </c>
+      <c r="K171" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11">
       <c r="A172">
         <v>1</v>
       </c>
@@ -6584,7 +7195,7 @@
         <v>113</v>
       </c>
       <c r="D172" t="s">
-        <v>660</v>
+        <v>635</v>
       </c>
       <c r="E172" t="s">
         <v>5</v>
@@ -6593,10 +7204,16 @@
         <v>151</v>
       </c>
       <c r="I172" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="173" spans="1:9">
+        <v>783</v>
+      </c>
+      <c r="J172" t="s">
+        <v>772</v>
+      </c>
+      <c r="K172" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11">
       <c r="A173">
         <v>1</v>
       </c>
@@ -6607,7 +7224,7 @@
         <v>114</v>
       </c>
       <c r="D173" t="s">
-        <v>650</v>
+        <v>876</v>
       </c>
       <c r="E173" t="s">
         <v>5</v>
@@ -6616,10 +7233,16 @@
         <v>153</v>
       </c>
       <c r="I173" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="174" spans="1:9">
+        <v>783</v>
+      </c>
+      <c r="J173" t="s">
+        <v>772</v>
+      </c>
+      <c r="K173" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11">
       <c r="A174">
         <v>1</v>
       </c>
@@ -6630,7 +7253,7 @@
         <v>115</v>
       </c>
       <c r="D174" t="s">
-        <v>649</v>
+        <v>636</v>
       </c>
       <c r="E174" t="s">
         <v>5</v>
@@ -6639,10 +7262,16 @@
         <v>155</v>
       </c>
       <c r="I174" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="175" spans="1:9">
+        <v>783</v>
+      </c>
+      <c r="J174" t="s">
+        <v>772</v>
+      </c>
+      <c r="K174" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11">
       <c r="A175">
         <v>1</v>
       </c>
@@ -6653,7 +7282,7 @@
         <v>116</v>
       </c>
       <c r="D175" t="s">
-        <v>665</v>
+        <v>877</v>
       </c>
       <c r="E175" t="s">
         <v>5</v>
@@ -6662,10 +7291,16 @@
         <v>157</v>
       </c>
       <c r="I175" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="176" spans="1:9">
+        <v>783</v>
+      </c>
+      <c r="J175" t="s">
+        <v>772</v>
+      </c>
+      <c r="K175" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11">
       <c r="A176">
         <v>1</v>
       </c>
@@ -6675,9 +7310,6 @@
       <c r="C176" s="3">
         <v>117</v>
       </c>
-      <c r="D176" t="s">
-        <v>664</v>
-      </c>
       <c r="E176" t="s">
         <v>5</v>
       </c>
@@ -6685,7 +7317,10 @@
         <v>159</v>
       </c>
       <c r="I176" t="s">
-        <v>767</v>
+        <v>783</v>
+      </c>
+      <c r="J176" t="s">
+        <v>772</v>
       </c>
     </row>
     <row r="177" spans="1:11">
@@ -6698,9 +7333,7 @@
       <c r="C177" s="3">
         <v>118</v>
       </c>
-      <c r="D177" t="s">
-        <v>635</v>
-      </c>
+      <c r="D177" s="4"/>
       <c r="E177" t="s">
         <v>5</v>
       </c>
@@ -6708,7 +7341,13 @@
         <v>161</v>
       </c>
       <c r="I177" t="s">
-        <v>767</v>
+        <v>783</v>
+      </c>
+      <c r="J177" t="s">
+        <v>772</v>
+      </c>
+      <c r="K177" t="s">
+        <v>841</v>
       </c>
     </row>
     <row r="178" spans="1:11">
@@ -6721,9 +7360,6 @@
       <c r="C178" s="3">
         <v>119</v>
       </c>
-      <c r="D178" t="s">
-        <v>634</v>
-      </c>
       <c r="E178" t="s">
         <v>5</v>
       </c>
@@ -6731,7 +7367,10 @@
         <v>163</v>
       </c>
       <c r="I178" t="s">
-        <v>767</v>
+        <v>783</v>
+      </c>
+      <c r="J178" t="s">
+        <v>772</v>
       </c>
     </row>
     <row r="179" spans="1:11">
@@ -6745,7 +7384,7 @@
         <v>0</v>
       </c>
       <c r="D179" t="s">
-        <v>654</v>
+        <v>647</v>
       </c>
       <c r="E179" t="s">
         <v>5</v>
@@ -6754,7 +7393,7 @@
         <v>361</v>
       </c>
       <c r="I179" t="s">
-        <v>766</v>
+        <v>755</v>
       </c>
     </row>
     <row r="180" spans="1:11">
@@ -6768,7 +7407,7 @@
         <v>1</v>
       </c>
       <c r="D180" t="s">
-        <v>666</v>
+        <v>659</v>
       </c>
       <c r="E180" t="s">
         <v>5</v>
@@ -6777,7 +7416,7 @@
         <v>373</v>
       </c>
       <c r="I180" t="s">
-        <v>766</v>
+        <v>755</v>
       </c>
     </row>
     <row r="181" spans="1:11">
@@ -6791,7 +7430,7 @@
         <v>2</v>
       </c>
       <c r="D181" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="E181" t="s">
         <v>5</v>
@@ -6800,7 +7439,7 @@
         <v>375</v>
       </c>
       <c r="I181" t="s">
-        <v>766</v>
+        <v>755</v>
       </c>
     </row>
     <row r="182" spans="1:11">
@@ -6814,7 +7453,7 @@
         <v>3</v>
       </c>
       <c r="D182" t="s">
-        <v>772</v>
+        <v>761</v>
       </c>
       <c r="E182" t="s">
         <v>5</v>
@@ -6823,7 +7462,7 @@
         <v>377</v>
       </c>
       <c r="I182" t="s">
-        <v>776</v>
+        <v>765</v>
       </c>
     </row>
     <row r="183" spans="1:11">
@@ -6837,7 +7476,7 @@
         <v>4</v>
       </c>
       <c r="D183" t="s">
-        <v>773</v>
+        <v>762</v>
       </c>
       <c r="E183" t="s">
         <v>5</v>
@@ -6846,7 +7485,7 @@
         <v>379</v>
       </c>
       <c r="I183" t="s">
-        <v>776</v>
+        <v>765</v>
       </c>
     </row>
     <row r="184" spans="1:11">
@@ -6860,7 +7499,7 @@
         <v>5</v>
       </c>
       <c r="D184" t="s">
-        <v>774</v>
+        <v>763</v>
       </c>
       <c r="E184" t="s">
         <v>5</v>
@@ -6869,7 +7508,7 @@
         <v>381</v>
       </c>
       <c r="I184" t="s">
-        <v>777</v>
+        <v>766</v>
       </c>
     </row>
     <row r="185" spans="1:11">
@@ -6883,7 +7522,7 @@
         <v>6</v>
       </c>
       <c r="D185" t="s">
-        <v>775</v>
+        <v>764</v>
       </c>
       <c r="E185" t="s">
         <v>5</v>
@@ -6892,7 +7531,7 @@
         <v>383</v>
       </c>
       <c r="I185" t="s">
-        <v>777</v>
+        <v>766</v>
       </c>
     </row>
     <row r="186" spans="1:11">
@@ -6906,7 +7545,7 @@
         <v>7</v>
       </c>
       <c r="D186" t="s">
-        <v>667</v>
+        <v>867</v>
       </c>
       <c r="E186" t="s">
         <v>5</v>
@@ -6915,7 +7554,10 @@
         <v>385</v>
       </c>
       <c r="I186" t="s">
-        <v>766</v>
+        <v>773</v>
+      </c>
+      <c r="K186">
+        <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:11">
@@ -6929,7 +7571,7 @@
         <v>8</v>
       </c>
       <c r="D187" t="s">
-        <v>641</v>
+        <v>868</v>
       </c>
       <c r="E187" t="s">
         <v>5</v>
@@ -6938,7 +7580,10 @@
         <v>387</v>
       </c>
       <c r="I187" t="s">
-        <v>766</v>
+        <v>755</v>
+      </c>
+      <c r="K187">
+        <v>0</v>
       </c>
     </row>
     <row r="188" spans="1:11">
@@ -6952,7 +7597,7 @@
         <v>9</v>
       </c>
       <c r="D188" t="s">
-        <v>631</v>
+        <v>869</v>
       </c>
       <c r="E188" t="s">
         <v>5</v>
@@ -6961,7 +7606,10 @@
         <v>389</v>
       </c>
       <c r="I188" t="s">
-        <v>766</v>
+        <v>755</v>
+      </c>
+      <c r="K188">
+        <v>0</v>
       </c>
     </row>
     <row r="189" spans="1:11">
@@ -6975,7 +7623,7 @@
         <v>10</v>
       </c>
       <c r="D189" t="s">
-        <v>639</v>
+        <v>870</v>
       </c>
       <c r="E189" t="s">
         <v>5</v>
@@ -6984,7 +7632,10 @@
         <v>363</v>
       </c>
       <c r="I189" t="s">
-        <v>766</v>
+        <v>755</v>
+      </c>
+      <c r="K189">
+        <v>0</v>
       </c>
     </row>
     <row r="190" spans="1:11">
@@ -6998,7 +7649,7 @@
         <v>11</v>
       </c>
       <c r="D190" t="s">
-        <v>620</v>
+        <v>871</v>
       </c>
       <c r="E190" t="s">
         <v>5</v>
@@ -7007,7 +7658,10 @@
         <v>365</v>
       </c>
       <c r="I190" t="s">
-        <v>766</v>
+        <v>755</v>
+      </c>
+      <c r="K190">
+        <v>1</v>
       </c>
     </row>
     <row r="191" spans="1:11">
@@ -7021,7 +7675,7 @@
         <v>12</v>
       </c>
       <c r="D191" t="s">
-        <v>603</v>
+        <v>872</v>
       </c>
       <c r="E191" t="s">
         <v>5</v>
@@ -7030,10 +7684,10 @@
         <v>367</v>
       </c>
       <c r="I191" t="s">
-        <v>766</v>
-      </c>
-      <c r="K191" t="s">
-        <v>763</v>
+        <v>755</v>
+      </c>
+      <c r="K191">
+        <v>1</v>
       </c>
     </row>
     <row r="192" spans="1:11">
@@ -7047,7 +7701,7 @@
         <v>13</v>
       </c>
       <c r="D192" t="s">
-        <v>593</v>
+        <v>873</v>
       </c>
       <c r="E192" t="s">
         <v>5</v>
@@ -7056,10 +7710,10 @@
         <v>369</v>
       </c>
       <c r="I192" t="s">
-        <v>766</v>
-      </c>
-      <c r="K192" t="s">
-        <v>764</v>
+        <v>755</v>
+      </c>
+      <c r="K192">
+        <v>1</v>
       </c>
     </row>
     <row r="193" spans="1:11">
@@ -7073,7 +7727,7 @@
         <v>14</v>
       </c>
       <c r="D193" t="s">
-        <v>595</v>
+        <v>874</v>
       </c>
       <c r="E193" t="s">
         <v>5</v>
@@ -7082,10 +7736,10 @@
         <v>371</v>
       </c>
       <c r="I193" t="s">
-        <v>766</v>
-      </c>
-      <c r="K193" t="s">
-        <v>765</v>
+        <v>755</v>
+      </c>
+      <c r="K193">
+        <v>0</v>
       </c>
     </row>
     <row r="194" spans="1:11">
@@ -7102,7 +7756,7 @@
         <v>391</v>
       </c>
       <c r="I194" t="s">
-        <v>762</v>
+        <v>754</v>
       </c>
     </row>
     <row r="195" spans="1:11">
@@ -7119,7 +7773,7 @@
         <v>393</v>
       </c>
       <c r="I195" t="s">
-        <v>762</v>
+        <v>754</v>
       </c>
     </row>
     <row r="196" spans="1:11">
@@ -7130,7 +7784,7 @@
         <v>394</v>
       </c>
       <c r="D196" t="s">
-        <v>656</v>
+        <v>649</v>
       </c>
       <c r="E196" t="s">
         <v>5</v>
@@ -7147,7 +7801,7 @@
         <v>396</v>
       </c>
       <c r="D197" t="s">
-        <v>782</v>
+        <v>771</v>
       </c>
       <c r="E197" t="s">
         <v>5</v>
@@ -7181,7 +7835,7 @@
         <v>400</v>
       </c>
       <c r="D199" t="s">
-        <v>781</v>
+        <v>770</v>
       </c>
       <c r="E199" t="s">
         <v>5</v>
@@ -7204,7 +7858,7 @@
         <v>403</v>
       </c>
       <c r="I200" t="s">
-        <v>762</v>
+        <v>754</v>
       </c>
     </row>
     <row r="201" spans="1:11">
@@ -7298,7 +7952,7 @@
         <v>418</v>
       </c>
       <c r="D208" t="s">
-        <v>702</v>
+        <v>694</v>
       </c>
       <c r="E208" t="s">
         <v>5</v>
@@ -7348,7 +8002,7 @@
         <v>426</v>
       </c>
       <c r="D212" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="E212" t="s">
         <v>5</v>
@@ -7399,7 +8053,7 @@
         <v>432</v>
       </c>
       <c r="D215" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="E215" t="s">
         <v>5</v>
@@ -7433,7 +8087,7 @@
         <v>436</v>
       </c>
       <c r="D217" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="E217" t="s">
         <v>5</v>
@@ -7450,7 +8104,7 @@
         <v>438</v>
       </c>
       <c r="D218" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="E218" t="s">
         <v>5</v>
@@ -7495,7 +8149,7 @@
         <v>444</v>
       </c>
       <c r="D221" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="E221" t="s">
         <v>5</v>
@@ -7512,7 +8166,7 @@
         <v>446</v>
       </c>
       <c r="D222" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="E222" t="s">
         <v>5</v>
@@ -7700,7 +8354,7 @@
         <v>478</v>
       </c>
       <c r="D238" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="E238" t="s">
         <v>5</v>
@@ -7717,7 +8371,7 @@
         <v>480</v>
       </c>
       <c r="D239" t="s">
-        <v>642</v>
+        <v>635</v>
       </c>
       <c r="E239" t="s">
         <v>5</v>
@@ -7910,7 +8564,7 @@
         <v>514</v>
       </c>
       <c r="D256" t="s">
-        <v>643</v>
+        <v>636</v>
       </c>
       <c r="E256" t="s">
         <v>5</v>
@@ -7927,7 +8581,7 @@
         <v>516</v>
       </c>
       <c r="D257" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="E257" t="s">
         <v>5</v>
@@ -7944,7 +8598,7 @@
         <v>518</v>
       </c>
       <c r="D258" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="E258" t="s">
         <v>5</v>
@@ -7961,7 +8615,7 @@
         <v>520</v>
       </c>
       <c r="D259" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="E259" t="s">
         <v>5</v>
@@ -7978,7 +8632,7 @@
         <v>522</v>
       </c>
       <c r="D260" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="E260" t="s">
         <v>5</v>
@@ -7995,7 +8649,7 @@
         <v>524</v>
       </c>
       <c r="D261" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="E261" t="s">
         <v>5</v>
@@ -8012,7 +8666,7 @@
         <v>526</v>
       </c>
       <c r="D262" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="E262" t="s">
         <v>5</v>
@@ -8029,7 +8683,7 @@
         <v>528</v>
       </c>
       <c r="D263" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="E263" t="s">
         <v>5</v>
@@ -8046,7 +8700,7 @@
         <v>530</v>
       </c>
       <c r="D264" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
       <c r="E264" t="s">
         <v>5</v>
@@ -8063,7 +8717,7 @@
         <v>532</v>
       </c>
       <c r="D265" t="s">
-        <v>693</v>
+        <v>685</v>
       </c>
       <c r="E265" t="s">
         <v>5</v>
@@ -8341,7 +8995,7 @@
         <v>582</v>
       </c>
       <c r="D290" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="E290" t="s">
         <v>5</v>
@@ -8355,7 +9009,7 @@
         <v>584</v>
       </c>
       <c r="D291" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="E291" t="s">
         <v>5</v>
@@ -8365,9 +9019,6 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="J148:L162">
-    <sortCondition ref="J148:J162"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -8375,10 +9026,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:A11"/>
+  <dimension ref="A3:A52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8388,47 +9039,247 @@
   <sheetData>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>708</v>
+        <v>700</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>720</v>
+        <v>712</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>721</v>
+        <v>713</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>726</v>
+        <v>718</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>727</v>
+        <v>719</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>734</v>
+        <v>726</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>735</v>
+        <v>727</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>739</v>
+        <v>731</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>655</v>
+        <v>648</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>629</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
After routing re-ordered A/D
</commit_message>
<xml_diff>
--- a/syscon_usb/DACS_V1_0_ISE/tools/dacs.ucf.xlsx
+++ b/syscon_usb/DACS_V1_0_ISE/tools/dacs.ucf.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2309" uniqueCount="905">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2311" uniqueCount="908">
   <si>
     <t>IOSTANDARD</t>
   </si>
@@ -2735,6 +2735,15 @@
   </si>
   <si>
     <t>844F</t>
+  </si>
+  <si>
+    <t>I/O Panel</t>
+  </si>
+  <si>
+    <t>Flight_OK</t>
+  </si>
+  <si>
+    <t>SPR_CPSW_S</t>
   </si>
 </sst>
 </file>
@@ -12528,7 +12537,7 @@
         <v>96</v>
       </c>
       <c r="D113" s="3">
-        <f t="shared" ref="D113:D144" si="4">FLOOR(C113/8,1)</f>
+        <f t="shared" ref="D113:D136" si="4">FLOOR(C113/8,1)</f>
         <v>12</v>
       </c>
       <c r="E113" t="s">
@@ -13296,11 +13305,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O217"/>
+  <dimension ref="A1:P217"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L154" sqref="L154"/>
+      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P152" sqref="P152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18967,7 +18976,7 @@
         <v/>
       </c>
     </row>
-    <row r="145" spans="1:15">
+    <row r="145" spans="1:16">
       <c r="A145" s="3">
         <v>1</v>
       </c>
@@ -19002,7 +19011,7 @@
         <v/>
       </c>
     </row>
-    <row r="146" spans="1:15">
+    <row r="146" spans="1:16">
       <c r="A146" s="3">
         <v>1</v>
       </c>
@@ -19037,7 +19046,7 @@
         <v/>
       </c>
     </row>
-    <row r="147" spans="1:15">
+    <row r="147" spans="1:16">
       <c r="A147" s="3">
         <v>1</v>
       </c>
@@ -19072,7 +19081,7 @@
         <v/>
       </c>
     </row>
-    <row r="148" spans="1:15">
+    <row r="148" spans="1:16">
       <c r="A148" s="3">
         <v>1</v>
       </c>
@@ -19107,7 +19116,7 @@
         <v/>
       </c>
     </row>
-    <row r="149" spans="1:15">
+    <row r="149" spans="1:16">
       <c r="A149" s="3">
         <v>1</v>
       </c>
@@ -19142,7 +19151,7 @@
         <v/>
       </c>
     </row>
-    <row r="150" spans="1:15">
+    <row r="150" spans="1:16">
       <c r="A150" s="3">
         <v>1</v>
       </c>
@@ -19179,8 +19188,11 @@
         <f t="shared" si="24"/>
         <v/>
       </c>
-    </row>
-    <row r="151" spans="1:15">
+      <c r="P150" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16">
       <c r="A151" s="3">
         <v>1</v>
       </c>
@@ -19217,8 +19229,11 @@
         <f t="shared" si="24"/>
         <v/>
       </c>
-    </row>
-    <row r="152" spans="1:15">
+      <c r="P151" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="152" spans="1:16">
       <c r="A152" s="3">
         <v>1</v>
       </c>
@@ -19249,14 +19264,14 @@
         <v>276</v>
       </c>
       <c r="L152" t="s">
-        <v>657</v>
+        <v>906</v>
       </c>
       <c r="N152" t="str">
         <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
-    <row r="153" spans="1:15">
+    <row r="153" spans="1:16">
       <c r="A153" s="3">
         <v>1</v>
       </c>
@@ -19287,14 +19302,14 @@
         <v>278</v>
       </c>
       <c r="L153" t="s">
-        <v>658</v>
+        <v>907</v>
       </c>
       <c r="N153" t="str">
         <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
-    <row r="154" spans="1:15">
+    <row r="154" spans="1:16">
       <c r="A154" s="3">
         <v>1</v>
       </c>
@@ -19335,7 +19350,7 @@
         <v>8440</v>
       </c>
     </row>
-    <row r="155" spans="1:15">
+    <row r="155" spans="1:16">
       <c r="A155" s="3">
         <v>1</v>
       </c>
@@ -19376,7 +19391,7 @@
         <v>8441</v>
       </c>
     </row>
-    <row r="156" spans="1:15">
+    <row r="156" spans="1:16">
       <c r="A156" s="3">
         <v>1</v>
       </c>
@@ -19417,7 +19432,7 @@
         <v>8442</v>
       </c>
     </row>
-    <row r="157" spans="1:15">
+    <row r="157" spans="1:16">
       <c r="A157" s="3">
         <v>1</v>
       </c>
@@ -19458,7 +19473,7 @@
         <v>8443</v>
       </c>
     </row>
-    <row r="158" spans="1:15">
+    <row r="158" spans="1:16">
       <c r="A158" s="3">
         <v>1</v>
       </c>
@@ -19499,7 +19514,7 @@
         <v>8444</v>
       </c>
     </row>
-    <row r="159" spans="1:15">
+    <row r="159" spans="1:16">
       <c r="A159" s="3">
         <v>1</v>
       </c>
@@ -19540,7 +19555,7 @@
         <v>8445</v>
       </c>
     </row>
-    <row r="160" spans="1:15">
+    <row r="160" spans="1:16">
       <c r="A160" s="3">
         <v>1</v>
       </c>
@@ -20870,7 +20885,7 @@
         <v>1</v>
       </c>
       <c r="I195" s="3">
-        <f t="shared" ref="I195:I258" si="34">I194+H195</f>
+        <f t="shared" ref="I195:I217" si="34">I194+H195</f>
         <v>22</v>
       </c>
       <c r="N195" t="str">

</xml_diff>

<commit_message>
Time for a commit
</commit_message>
<xml_diff>
--- a/syscon_usb/DACS_V1_0_ISE/tools/dacs.ucf.xlsx
+++ b/syscon_usb/DACS_V1_0_ISE/tools/dacs.ucf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="19035" windowHeight="12015" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="19035" windowHeight="12015" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Board" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2311" uniqueCount="908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2311" uniqueCount="909">
   <si>
     <t>IOSTANDARD</t>
   </si>
@@ -2744,6 +2744,9 @@
   </si>
   <si>
     <t>SPR_CPSW_S</t>
+  </si>
+  <si>
+    <t>not Cmd&lt;24&gt;</t>
   </si>
 </sst>
 </file>
@@ -9199,9 +9202,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E137" sqref="E137"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9703,7 +9706,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>767</v>
+        <v>908</v>
       </c>
       <c r="F17" t="s">
         <v>5</v>
@@ -13307,8 +13310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P217"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P152" sqref="P152"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
List of DACS boards and modification history HTW definitions.
</commit_message>
<xml_diff>
--- a/syscon_usb/DACS_V1_0_ISE/tools/dacs.ucf.xlsx
+++ b/syscon_usb/DACS_V1_0_ISE/tools/dacs.ucf.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2931" uniqueCount="1008">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2959" uniqueCount="1022">
   <si>
     <t>IOSTANDARD</t>
   </si>
@@ -3046,6 +3046,48 @@
   </si>
   <si>
     <t>spare</t>
+  </si>
+  <si>
+    <t>Scroll_Pump</t>
+  </si>
+  <si>
+    <t>Cal_Bub1_Vlv</t>
+  </si>
+  <si>
+    <t>Cal_Bub2_Vlv</t>
+  </si>
+  <si>
+    <t>TE_HC1</t>
+  </si>
+  <si>
+    <t>LPV_HC</t>
+  </si>
+  <si>
+    <t>Cell_HC</t>
+  </si>
+  <si>
+    <t>DPV_HC</t>
+  </si>
+  <si>
+    <t>SpCmd1</t>
+  </si>
+  <si>
+    <t>SpCmd2</t>
+  </si>
+  <si>
+    <t>L1Cmd</t>
+  </si>
+  <si>
+    <t>TE_HC2</t>
+  </si>
+  <si>
+    <t>Gas_Vlv</t>
+  </si>
+  <si>
+    <t>Edw_Vlv</t>
+  </si>
+  <si>
+    <t>Bub_Gas_Vlv</t>
   </si>
 </sst>
 </file>
@@ -3795,6 +3837,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3807,12 +3855,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -9893,7 +9935,7 @@
   <dimension ref="A1:S137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="I29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="I75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="O14" sqref="O14"/>
@@ -9920,20 +9962,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="55" t="s">
         <v>745</v>
       </c>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51" t="s">
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55" t="s">
         <v>908</v>
       </c>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
     </row>
     <row r="2" spans="1:19">
       <c r="B2" s="1" t="s">
@@ -12067,7 +12109,7 @@
       <c r="N50" s="7" t="s">
         <v>962</v>
       </c>
-      <c r="O50" s="55" t="s">
+      <c r="O50" s="51" t="s">
         <v>862</v>
       </c>
       <c r="P50" s="37"/>
@@ -12112,7 +12154,7 @@
       <c r="N51" s="7" t="s">
         <v>962</v>
       </c>
-      <c r="O51" s="55" t="s">
+      <c r="O51" s="51" t="s">
         <v>863</v>
       </c>
       <c r="P51" s="37"/>
@@ -12157,7 +12199,7 @@
       <c r="N52" s="7" t="s">
         <v>962</v>
       </c>
-      <c r="O52" s="55" t="s">
+      <c r="O52" s="51" t="s">
         <v>864</v>
       </c>
       <c r="P52" s="37"/>
@@ -12199,7 +12241,7 @@
       <c r="N53" s="7" t="s">
         <v>962</v>
       </c>
-      <c r="O53" s="55" t="s">
+      <c r="O53" s="51" t="s">
         <v>865</v>
       </c>
       <c r="P53" s="37"/>
@@ -12238,7 +12280,7 @@
       <c r="N54" s="3" t="s">
         <v>950</v>
       </c>
-      <c r="O54" s="56" t="s">
+      <c r="O54" s="52" t="s">
         <v>866</v>
       </c>
       <c r="P54" s="37"/>
@@ -12277,7 +12319,7 @@
       <c r="N55" s="3" t="s">
         <v>950</v>
       </c>
-      <c r="O55" s="56" t="s">
+      <c r="O55" s="52" t="s">
         <v>867</v>
       </c>
       <c r="P55" s="37"/>
@@ -12316,7 +12358,7 @@
       <c r="N56" s="3" t="s">
         <v>950</v>
       </c>
-      <c r="O56" s="56" t="s">
+      <c r="O56" s="52" t="s">
         <v>993</v>
       </c>
       <c r="P56" s="37"/>
@@ -12355,7 +12397,7 @@
       <c r="N57" s="3" t="s">
         <v>950</v>
       </c>
-      <c r="O57" s="56" t="s">
+      <c r="O57" s="52" t="s">
         <v>994</v>
       </c>
       <c r="P57" s="37"/>
@@ -16148,7 +16190,7 @@
       <c r="N137" s="21" t="s">
         <v>950</v>
       </c>
-      <c r="O137" s="57" t="s">
+      <c r="O137" s="53" t="s">
         <v>1000</v>
       </c>
       <c r="P137" s="22"/>
@@ -16178,8 +16220,8 @@
   <dimension ref="A1:AA218"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V195" sqref="V195"/>
+      <pane ySplit="2" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U61" sqref="U61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16208,32 +16250,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="56" t="s">
         <v>745</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="53" t="s">
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="57" t="s">
         <v>908</v>
       </c>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
+      <c r="Z1" s="58"/>
+      <c r="AA1" s="58"/>
     </row>
     <row r="2" spans="1:27">
       <c r="A2" s="2" t="s">
@@ -16369,7 +16411,7 @@
         <v>965</v>
       </c>
       <c r="Y3" t="str">
-        <f t="shared" ref="Y3:Z66" si="3">IF(S3,CONCATENATE("dig_io_nc(",T3,")"),"")</f>
+        <f t="shared" ref="Y3:Y66" si="3">IF(S3,CONCATENATE("dig_io_nc(",T3,")"),"")</f>
         <v/>
       </c>
       <c r="Z3" t="str">
@@ -17827,7 +17869,7 @@
         <v>0</v>
       </c>
       <c r="S27" s="3">
-        <f t="shared" ref="S3:S66" si="12">IF(AND(ISBLANK(U27), ISBLANK(V27)),1,0)</f>
+        <f t="shared" ref="S27:S66" si="12">IF(AND(ISBLANK(U27), ISBLANK(V27)),1,0)</f>
         <v>0</v>
       </c>
       <c r="T27" s="3">
@@ -17838,6 +17880,9 @@
         <f>CONCATENATE("Cmd_",R27,"_On")</f>
         <v>Cmd_0_On</v>
       </c>
+      <c r="X27" t="s">
+        <v>1008</v>
+      </c>
       <c r="Y27" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -17909,6 +17954,9 @@
         <f>CONCATENATE("Cmd_",R28,"_Off")</f>
         <v>Cmd_0_Off</v>
       </c>
+      <c r="X28" t="s">
+        <v>1008</v>
+      </c>
       <c r="Y28" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -17980,6 +18028,9 @@
         <f>CONCATENATE("Cmd_",R29,"_On")</f>
         <v>Cmd_1_On</v>
       </c>
+      <c r="X29" t="s">
+        <v>1009</v>
+      </c>
       <c r="Y29" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -18051,6 +18102,9 @@
         <f>CONCATENATE("Cmd_",R30,"_Off")</f>
         <v>Cmd_1_Off</v>
       </c>
+      <c r="X30" t="s">
+        <v>1009</v>
+      </c>
       <c r="Y30" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -18121,6 +18175,9 @@
         <f>CONCATENATE("Cmd_",R31,"_On")</f>
         <v>Cmd_2_On</v>
       </c>
+      <c r="X31" t="s">
+        <v>1010</v>
+      </c>
       <c r="Y31" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -18191,6 +18248,9 @@
         <f>CONCATENATE("Cmd_",R32,"_Off")</f>
         <v>Cmd_2_Off</v>
       </c>
+      <c r="X32" t="s">
+        <v>1010</v>
+      </c>
       <c r="Y32" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -18261,6 +18321,9 @@
         <f>CONCATENATE("Cmd_",R33,"_On")</f>
         <v>Cmd_3_On</v>
       </c>
+      <c r="X33" t="s">
+        <v>1011</v>
+      </c>
       <c r="Y33" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -18331,6 +18394,9 @@
         <f>CONCATENATE("Cmd_",R34,"_Off")</f>
         <v>Cmd_3_Off</v>
       </c>
+      <c r="X34" t="s">
+        <v>1011</v>
+      </c>
       <c r="Y34" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -18401,6 +18467,9 @@
         <f>CONCATENATE("Cmd_",R35,"_On")</f>
         <v>Cmd_4_On</v>
       </c>
+      <c r="X35" t="s">
+        <v>1012</v>
+      </c>
       <c r="Y35" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -18471,6 +18540,9 @@
         <f>CONCATENATE("Cmd_",R36,"_Off")</f>
         <v>Cmd_4_Off</v>
       </c>
+      <c r="X36" t="s">
+        <v>1012</v>
+      </c>
       <c r="Y36" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -18541,6 +18613,9 @@
         <f>CONCATENATE("Cmd_",R37,"_On")</f>
         <v>Cmd_5_On</v>
       </c>
+      <c r="X37" t="s">
+        <v>1013</v>
+      </c>
       <c r="Y37" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -18611,6 +18686,9 @@
         <f>CONCATENATE("Cmd_",R38,"_Off")</f>
         <v>Cmd_5_Off</v>
       </c>
+      <c r="X38" t="s">
+        <v>1013</v>
+      </c>
       <c r="Y38" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -18681,6 +18759,9 @@
         <f>CONCATENATE("Cmd_",R39,"_On")</f>
         <v>Cmd_6_On</v>
       </c>
+      <c r="X39" t="s">
+        <v>1014</v>
+      </c>
       <c r="Y39" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -18751,6 +18832,9 @@
         <f>CONCATENATE("Cmd_",R40,"_Off")</f>
         <v>Cmd_6_Off</v>
       </c>
+      <c r="X40" t="s">
+        <v>1014</v>
+      </c>
       <c r="Y40" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -18821,6 +18905,9 @@
         <f>CONCATENATE("Cmd_",R41,"_On")</f>
         <v>Cmd_7_On</v>
       </c>
+      <c r="X41" t="s">
+        <v>1015</v>
+      </c>
       <c r="Y41" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -18891,6 +18978,9 @@
         <f>CONCATENATE("Cmd_",R42,"_Off")</f>
         <v>Cmd_7_Off</v>
       </c>
+      <c r="X42" t="s">
+        <v>1015</v>
+      </c>
       <c r="Y42" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -18961,6 +19051,9 @@
         <f>CONCATENATE("Cmd_",R43,"_On")</f>
         <v>Cmd_8_On</v>
       </c>
+      <c r="X43" t="s">
+        <v>1016</v>
+      </c>
       <c r="Y43" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -19031,6 +19124,9 @@
         <f>CONCATENATE("Cmd_",R44,"_Off")</f>
         <v>Cmd_8_Off</v>
       </c>
+      <c r="X44" t="s">
+        <v>1016</v>
+      </c>
       <c r="Y44" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -19101,6 +19197,9 @@
         <f>CONCATENATE("Cmd_",R45,"_On")</f>
         <v>Cmd_9_On</v>
       </c>
+      <c r="X45" t="s">
+        <v>1017</v>
+      </c>
       <c r="Y45" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -19171,6 +19270,9 @@
         <f>CONCATENATE("Cmd_",R46,"_Off")</f>
         <v>Cmd_9_Off</v>
       </c>
+      <c r="X46" t="s">
+        <v>1017</v>
+      </c>
       <c r="Y46" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -19241,6 +19343,9 @@
         <f>CONCATENATE("Cmd_",R47,"_On")</f>
         <v>Cmd_10_On</v>
       </c>
+      <c r="X47" t="s">
+        <v>1018</v>
+      </c>
       <c r="Y47" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -19311,6 +19416,9 @@
         <f>CONCATENATE("Cmd_",R48,"_Off")</f>
         <v>Cmd_10_Off</v>
       </c>
+      <c r="X48" t="s">
+        <v>1018</v>
+      </c>
       <c r="Y48" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -19381,6 +19489,9 @@
         <f>CONCATENATE("Cmd_",R49,"_On")</f>
         <v>Cmd_11_On</v>
       </c>
+      <c r="X49" t="s">
+        <v>1019</v>
+      </c>
       <c r="Y49" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -19451,6 +19562,9 @@
         <f>CONCATENATE("Cmd_",R50,"_Off")</f>
         <v>Cmd_11_Off</v>
       </c>
+      <c r="X50" t="s">
+        <v>1019</v>
+      </c>
       <c r="Y50" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -19521,6 +19635,9 @@
         <f>CONCATENATE("Cmd_",R51,"_On")</f>
         <v>Cmd_12_On</v>
       </c>
+      <c r="X51" t="s">
+        <v>1020</v>
+      </c>
       <c r="Y51" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -19591,6 +19708,9 @@
         <f>CONCATENATE("Cmd_",R52,"_Off")</f>
         <v>Cmd_12_Off</v>
       </c>
+      <c r="X52" t="s">
+        <v>1020</v>
+      </c>
       <c r="Y52" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -19661,6 +19781,9 @@
         <f>CONCATENATE("Cmd_",R53,"_On")</f>
         <v>Cmd_13_On</v>
       </c>
+      <c r="X53" t="s">
+        <v>1021</v>
+      </c>
       <c r="Y53" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -19731,6 +19854,9 @@
         <f>CONCATENATE("Cmd_",R54,"_Off")</f>
         <v>Cmd_13_Off</v>
       </c>
+      <c r="X54" t="s">
+        <v>1021</v>
+      </c>
       <c r="Y54" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -29432,7 +29558,7 @@
         <f t="shared" si="40"/>
         <v>1</v>
       </c>
-      <c r="V195" s="58" t="s">
+      <c r="V195" s="54" t="s">
         <v>244</v>
       </c>
       <c r="Y195" t="str">

</xml_diff>

<commit_message>
DACS Tool Updated documentation
</commit_message>
<xml_diff>
--- a/syscon_usb/DACS_V1_0_ISE/tools/dacs.ucf.xlsx
+++ b/syscon_usb/DACS_V1_0_ISE/tools/dacs.ucf.xlsx
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Board!$J$148:$J$162</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" calcMode="manual"/>
 </workbook>
 </file>
 
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3711" uniqueCount="1276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3711" uniqueCount="1282">
   <si>
     <t>IOSTANDARD</t>
   </si>
@@ -3503,12 +3503,6 @@
     <t>ILTEC_DS</t>
   </si>
   <si>
-    <t>L1_DS</t>
-  </si>
-  <si>
-    <t>L2_DS</t>
-  </si>
-  <si>
     <t>MM_Pump_DS</t>
   </si>
   <si>
@@ -3888,6 +3882,30 @@
   </si>
   <si>
     <t>DIO_2Sp/Coolant Divert</t>
+  </si>
+  <si>
+    <t>CoolPump_DS</t>
+  </si>
+  <si>
+    <t>InverterArm_DS</t>
+  </si>
+  <si>
+    <t>CoolantPump_Off</t>
+  </si>
+  <si>
+    <t>CoolantPump_On</t>
+  </si>
+  <si>
+    <t>ILTEC_On</t>
+  </si>
+  <si>
+    <t>ILTEC_Off</t>
+  </si>
+  <si>
+    <t>InverterArm_On</t>
+  </si>
+  <si>
+    <t>InverterArm_Off</t>
   </si>
 </sst>
 </file>
@@ -10699,7 +10717,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>919</v>
@@ -10708,7 +10726,7 @@
         <v>1031</v>
       </c>
       <c r="E2" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -10716,7 +10734,7 @@
         <v>56</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>920</v>
@@ -10725,7 +10743,7 @@
         <v>1032</v>
       </c>
       <c r="E3" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -10733,7 +10751,7 @@
         <v>58</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="C4" s="26" t="s">
         <v>921</v>
@@ -10742,7 +10760,7 @@
         <v>1033</v>
       </c>
       <c r="E4" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -10750,7 +10768,7 @@
         <v>60</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="C5" s="26" t="s">
         <v>922</v>
@@ -10759,7 +10777,7 @@
         <v>1034</v>
       </c>
       <c r="E5" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -10774,7 +10792,7 @@
         <v>1035</v>
       </c>
       <c r="E6" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -10789,7 +10807,7 @@
         <v>1036</v>
       </c>
       <c r="E7" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -10802,7 +10820,7 @@
         <v>1037</v>
       </c>
       <c r="E8" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -10815,7 +10833,7 @@
         <v>1038</v>
       </c>
       <c r="E9" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -10823,13 +10841,13 @@
         <v>70</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -10837,13 +10855,13 @@
         <v>72</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -10852,10 +10870,10 @@
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="72" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -10864,10 +10882,10 @@
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="72" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -10876,10 +10894,10 @@
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="72" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -10888,10 +10906,10 @@
       </c>
       <c r="B15" s="25"/>
       <c r="C15" s="72" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -11079,7 +11097,7 @@
       </c>
       <c r="R3" s="36"/>
       <c r="S3" s="52" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="T3" s="53" t="s">
         <v>958</v>
@@ -11465,7 +11483,7 @@
         <v>1</v>
       </c>
       <c r="R10" s="14" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="S10" s="45" t="s">
         <v>1125</v>
@@ -11916,7 +11934,7 @@
         <v>959</v>
       </c>
       <c r="R18" s="14" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="S18" s="32" t="s">
         <v>1039</v>
@@ -11973,7 +11991,7 @@
         <v>959</v>
       </c>
       <c r="R19" s="14" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="S19" s="32" t="s">
         <v>1040</v>
@@ -12030,7 +12048,7 @@
         <v>959</v>
       </c>
       <c r="R20" s="14" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="S20" s="32" t="s">
         <v>1041</v>
@@ -12087,7 +12105,7 @@
         <v>959</v>
       </c>
       <c r="R21" s="14" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="S21" s="32" t="s">
         <v>1042</v>
@@ -12144,7 +12162,7 @@
         <v>959</v>
       </c>
       <c r="R22" s="14" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="S22" s="32" t="s">
         <v>1043</v>
@@ -12201,7 +12219,7 @@
         <v>959</v>
       </c>
       <c r="R23" s="14" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="S23" s="32" t="s">
         <v>1044</v>
@@ -12258,7 +12276,7 @@
         <v>959</v>
       </c>
       <c r="R24" s="14" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="S24" s="32" t="s">
         <v>1045</v>
@@ -12762,7 +12780,7 @@
         <v>960</v>
       </c>
       <c r="R34" s="14" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="S34" s="32" t="s">
         <v>1054</v>
@@ -12813,7 +12831,7 @@
         <v>960</v>
       </c>
       <c r="R35" s="14" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="S35" s="32" t="s">
         <v>942</v>
@@ -12966,7 +12984,7 @@
         <v>960</v>
       </c>
       <c r="R38" s="14" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="S38" s="32" t="s">
         <v>1055</v>
@@ -13017,7 +13035,7 @@
         <v>960</v>
       </c>
       <c r="R39" s="14" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="S39" s="32" t="s">
         <v>1056</v>
@@ -13223,7 +13241,7 @@
         <v>949</v>
       </c>
       <c r="R43" s="14" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="S43" s="32" t="s">
         <v>1060</v>
@@ -13272,7 +13290,7 @@
         <v>949</v>
       </c>
       <c r="R44" s="14" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="S44" s="32" t="s">
         <v>1061</v>
@@ -13321,7 +13339,7 @@
         <v>949</v>
       </c>
       <c r="R45" s="14" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="S45" s="32" t="s">
         <v>1062</v>
@@ -14314,10 +14332,10 @@
         <v>949</v>
       </c>
       <c r="R64" s="14" t="s">
+        <v>1201</v>
+      </c>
+      <c r="S64" s="32" t="s">
         <v>1203</v>
-      </c>
-      <c r="S64" s="32" t="s">
-        <v>1205</v>
       </c>
       <c r="T64" s="31">
         <v>0</v>
@@ -14365,10 +14383,10 @@
         <v>949</v>
       </c>
       <c r="R65" s="14" t="s">
+        <v>1202</v>
+      </c>
+      <c r="S65" s="32" t="s">
         <v>1204</v>
-      </c>
-      <c r="S65" s="32" t="s">
-        <v>1206</v>
       </c>
       <c r="T65" s="31">
         <v>0</v>
@@ -14784,7 +14802,7 @@
         <v>949</v>
       </c>
       <c r="R74" s="14" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="S74" s="32" t="s">
         <v>1085</v>
@@ -14835,7 +14853,7 @@
         <v>949</v>
       </c>
       <c r="R75" s="14" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="S75" s="32" t="s">
         <v>1086</v>
@@ -14886,7 +14904,7 @@
         <v>949</v>
       </c>
       <c r="R76" s="14" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="S76" s="32" t="s">
         <v>1087</v>
@@ -14937,7 +14955,7 @@
         <v>949</v>
       </c>
       <c r="R77" s="14" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="S77" s="32" t="s">
         <v>1088</v>
@@ -14997,7 +15015,7 @@
         <v>963</v>
       </c>
       <c r="R78" s="14" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="S78" s="6" t="s">
         <v>1091</v>
@@ -15057,7 +15075,7 @@
         <v>963</v>
       </c>
       <c r="R79" s="14" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="S79" s="6" t="s">
         <v>1092</v>
@@ -15117,7 +15135,7 @@
         <v>963</v>
       </c>
       <c r="R80" s="14" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="S80" s="6" t="s">
         <v>1093</v>
@@ -15177,7 +15195,7 @@
         <v>963</v>
       </c>
       <c r="R81" s="14" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="S81" s="6" t="s">
         <v>1094</v>
@@ -17757,7 +17775,7 @@
         <v>949</v>
       </c>
       <c r="R124" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="S124" t="s">
         <v>701</v>
@@ -17817,7 +17835,7 @@
         <v>949</v>
       </c>
       <c r="R125" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="S125" t="s">
         <v>702</v>
@@ -18414,7 +18432,7 @@
         <v>780</v>
       </c>
       <c r="S135" s="6" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="T135" s="31">
         <v>0</v>
@@ -18532,7 +18550,7 @@
         <v>781</v>
       </c>
       <c r="S137" s="70" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="T137" s="48">
         <v>0</v>
@@ -18564,10 +18582,10 @@
   <dimension ref="A1:AL272"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AA120" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="AA128" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F2" sqref="F1:F1048576"/>
       <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
-      <selection pane="bottomRight" activeCell="AI133" sqref="AI133"/>
+      <selection pane="bottomRight" activeCell="AI145" sqref="AI145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22288,7 +22306,7 @@
       <c r="AG45" s="32"/>
       <c r="AH45" s="32"/>
       <c r="AI45" s="6" t="s">
-        <v>1101</v>
+        <v>1278</v>
       </c>
       <c r="AJ45" s="32"/>
       <c r="AK45" s="57"/>
@@ -22389,7 +22407,7 @@
       <c r="AG46" s="32"/>
       <c r="AH46" s="32"/>
       <c r="AI46" s="6" t="s">
-        <v>1101</v>
+        <v>1279</v>
       </c>
       <c r="AJ46" s="32"/>
       <c r="AK46" s="57"/>
@@ -22490,7 +22508,7 @@
       <c r="AG47" s="32"/>
       <c r="AH47" s="32"/>
       <c r="AI47" s="6" t="s">
-        <v>1102</v>
+        <v>1277</v>
       </c>
       <c r="AJ47" s="32"/>
       <c r="AK47" s="57"/>
@@ -22591,7 +22609,7 @@
       <c r="AG48" s="32"/>
       <c r="AH48" s="32"/>
       <c r="AI48" s="6" t="s">
-        <v>1102</v>
+        <v>1276</v>
       </c>
       <c r="AJ48" s="32"/>
       <c r="AK48" s="57"/>
@@ -22692,7 +22710,7 @@
       <c r="AG49" s="32"/>
       <c r="AH49" s="32"/>
       <c r="AI49" s="6" t="s">
-        <v>1103</v>
+        <v>1280</v>
       </c>
       <c r="AJ49" s="32"/>
       <c r="AK49" s="57"/>
@@ -22793,7 +22811,7 @@
       <c r="AG50" s="32"/>
       <c r="AH50" s="32"/>
       <c r="AI50" s="6" t="s">
-        <v>1103</v>
+        <v>1281</v>
       </c>
       <c r="AJ50" s="32"/>
       <c r="AK50" s="57"/>
@@ -30828,7 +30846,7 @@
       <c r="AG129" s="32"/>
       <c r="AH129" s="32"/>
       <c r="AI129" s="32" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="AJ129" s="32" t="str">
         <f t="shared" ref="AJ129:AJ192" si="200">IF(AD129,CONCATENATE("dig_io_nc(",AE129,")"),"")</f>
@@ -30925,7 +30943,7 @@
       <c r="AG130" s="32"/>
       <c r="AH130" s="32"/>
       <c r="AI130" s="32" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="AJ130" s="32" t="str">
         <f t="shared" si="200"/>
@@ -31022,7 +31040,7 @@
       <c r="AG131" s="32"/>
       <c r="AH131" s="32"/>
       <c r="AI131" s="32" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="AJ131" s="32" t="str">
         <f t="shared" si="200"/>
@@ -31119,7 +31137,7 @@
       <c r="AG132" s="32"/>
       <c r="AH132" s="32"/>
       <c r="AI132" s="32" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="AJ132" s="32" t="str">
         <f t="shared" si="200"/>
@@ -31212,7 +31230,7 @@
       </c>
       <c r="AH133" s="32"/>
       <c r="AI133" s="32" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="AJ133" s="32" t="str">
         <f t="shared" si="200"/>
@@ -31398,7 +31416,7 @@
       </c>
       <c r="AH135" s="32"/>
       <c r="AI135" s="6" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="AJ135" s="32" t="str">
         <f t="shared" si="200"/>
@@ -31491,7 +31509,7 @@
       </c>
       <c r="AH136" s="32"/>
       <c r="AI136" s="71" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="AJ136" s="32" t="str">
         <f t="shared" si="200"/>
@@ -31588,7 +31606,7 @@
       <c r="AG137" s="32"/>
       <c r="AH137" s="32"/>
       <c r="AI137" s="6" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="AJ137" s="32" t="str">
         <f t="shared" si="200"/>
@@ -32251,7 +32269,7 @@
       <c r="AG144" s="32"/>
       <c r="AH144" s="32"/>
       <c r="AI144" s="6" t="s">
-        <v>1147</v>
+        <v>1274</v>
       </c>
       <c r="AJ144" s="32" t="str">
         <f t="shared" si="200"/>
@@ -32350,7 +32368,7 @@
       <c r="AG145" s="32"/>
       <c r="AH145" s="32"/>
       <c r="AI145" s="6" t="s">
-        <v>1148</v>
+        <v>1275</v>
       </c>
       <c r="AJ145" s="32" t="str">
         <f t="shared" si="200"/>
@@ -32449,7 +32467,7 @@
       <c r="AG146" s="32"/>
       <c r="AH146" s="32"/>
       <c r="AI146" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="AJ146" s="32" t="str">
         <f t="shared" si="200"/>
@@ -32548,7 +32566,7 @@
       <c r="AG147" s="32"/>
       <c r="AH147" s="32"/>
       <c r="AI147" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="AJ147" s="32" t="str">
         <f t="shared" si="200"/>
@@ -32647,7 +32665,7 @@
       <c r="AG148" s="32"/>
       <c r="AH148" s="32"/>
       <c r="AI148" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="AJ148" s="32" t="str">
         <f t="shared" si="200"/>
@@ -32746,7 +32764,7 @@
       <c r="AG149" s="32"/>
       <c r="AH149" s="32"/>
       <c r="AI149" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="AJ149" s="32" t="str">
         <f t="shared" si="200"/>
@@ -32844,7 +32862,7 @@
       <c r="AG150" s="32"/>
       <c r="AH150" s="32"/>
       <c r="AI150" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="AJ150" s="32" t="str">
         <f t="shared" si="200"/>
@@ -32937,7 +32955,7 @@
       <c r="AG151" s="32"/>
       <c r="AH151" s="32"/>
       <c r="AI151" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="AJ151" s="32" t="str">
         <f t="shared" si="200"/>
@@ -33030,7 +33048,7 @@
       <c r="AG152" s="32"/>
       <c r="AH152" s="32"/>
       <c r="AI152" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="AJ152" s="32" t="str">
         <f t="shared" si="200"/>
@@ -33123,7 +33141,7 @@
       <c r="AG153" s="32"/>
       <c r="AH153" s="32"/>
       <c r="AI153" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="AJ153" s="32" t="str">
         <f t="shared" si="200"/>
@@ -33216,7 +33234,7 @@
       <c r="AG154" s="32"/>
       <c r="AH154" s="32"/>
       <c r="AI154" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="AJ154" s="32" t="str">
         <f t="shared" si="200"/>
@@ -33309,7 +33327,7 @@
       <c r="AG155" s="32"/>
       <c r="AH155" s="32"/>
       <c r="AI155" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="AJ155" s="32" t="str">
         <f t="shared" si="200"/>
@@ -33402,7 +33420,7 @@
       <c r="AG156" s="32"/>
       <c r="AH156" s="32"/>
       <c r="AI156" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="AJ156" s="32" t="str">
         <f t="shared" si="200"/>
@@ -33500,7 +33518,7 @@
       <c r="AG157" s="32"/>
       <c r="AH157" s="32"/>
       <c r="AI157" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="AJ157" s="32" t="str">
         <f t="shared" si="200"/>
@@ -33598,7 +33616,7 @@
       <c r="AG158" s="32"/>
       <c r="AH158" s="32"/>
       <c r="AI158" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="AJ158" s="32" t="str">
         <f t="shared" si="200"/>
@@ -33696,7 +33714,7 @@
       <c r="AG159" s="32"/>
       <c r="AH159" s="32"/>
       <c r="AI159" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="AJ159" s="32" t="str">
         <f t="shared" si="200"/>
@@ -33794,7 +33812,7 @@
       <c r="AG160" s="32"/>
       <c r="AH160" s="32"/>
       <c r="AI160" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="AJ160" s="32" t="str">
         <f t="shared" si="200"/>
@@ -33897,7 +33915,7 @@
       <c r="AG161" s="32"/>
       <c r="AH161" s="32"/>
       <c r="AI161" s="32" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="AJ161" s="32" t="str">
         <f t="shared" si="200"/>
@@ -34000,7 +34018,7 @@
       <c r="AG162" s="32"/>
       <c r="AH162" s="32"/>
       <c r="AI162" s="32" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="AJ162" s="32" t="str">
         <f t="shared" si="200"/>
@@ -34103,7 +34121,7 @@
       <c r="AG163" s="32"/>
       <c r="AH163" s="32"/>
       <c r="AI163" s="32" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="AJ163" s="32" t="str">
         <f t="shared" si="200"/>
@@ -34206,7 +34224,7 @@
       <c r="AG164" s="32"/>
       <c r="AH164" s="32"/>
       <c r="AI164" s="32" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="AJ164" s="32" t="str">
         <f t="shared" si="200"/>
@@ -34309,7 +34327,7 @@
       <c r="AG165" s="32"/>
       <c r="AH165" s="32"/>
       <c r="AI165" s="32" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="AJ165" s="32" t="str">
         <f t="shared" si="200"/>
@@ -34412,7 +34430,7 @@
       <c r="AG166" s="32"/>
       <c r="AH166" s="32"/>
       <c r="AI166" s="32" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="AJ166" s="32" t="str">
         <f t="shared" si="200"/>
@@ -34515,7 +34533,7 @@
       <c r="AG167" s="32"/>
       <c r="AH167" s="32"/>
       <c r="AI167" s="32" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="AJ167" s="32" t="str">
         <f t="shared" si="200"/>
@@ -34618,7 +34636,7 @@
       <c r="AG168" s="32"/>
       <c r="AH168" s="32"/>
       <c r="AI168" s="32" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="AJ168" s="32" t="str">
         <f t="shared" si="200"/>
@@ -34720,7 +34738,7 @@
       </c>
       <c r="AG169" s="32"/>
       <c r="AI169" s="32" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="AJ169" s="32" t="str">
         <f t="shared" si="200"/>
@@ -34924,7 +34942,7 @@
       </c>
       <c r="AG171" s="32"/>
       <c r="AI171" s="32" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="AJ171" s="32" t="str">
         <f t="shared" si="200"/>
@@ -35026,7 +35044,7 @@
       </c>
       <c r="AG172" s="32"/>
       <c r="AI172" s="32" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="AJ172" s="32" t="str">
         <f t="shared" si="200"/>
@@ -35128,7 +35146,7 @@
       </c>
       <c r="AG173" s="32"/>
       <c r="AI173" s="32" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="AJ173" s="32" t="str">
         <f t="shared" si="200"/>
@@ -35230,7 +35248,7 @@
       </c>
       <c r="AG174" s="32"/>
       <c r="AI174" s="32" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="AJ174" s="32" t="str">
         <f t="shared" si="200"/>
@@ -35332,7 +35350,7 @@
       </c>
       <c r="AG175" s="32"/>
       <c r="AI175" s="32" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="AJ175" s="32" t="str">
         <f t="shared" si="200"/>
@@ -35439,7 +35457,7 @@
       <c r="AG176" s="19"/>
       <c r="AH176" s="19"/>
       <c r="AI176" s="19" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="AJ176" s="32" t="str">
         <f t="shared" si="200"/>
@@ -35541,7 +35559,7 @@
       </c>
       <c r="AG177" s="32"/>
       <c r="AI177" s="32" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="AJ177" s="32" t="str">
         <f t="shared" si="200"/>
@@ -35643,7 +35661,7 @@
       </c>
       <c r="AG178" s="32"/>
       <c r="AI178" s="32" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="AJ178" s="32" t="str">
         <f t="shared" si="200"/>
@@ -35745,7 +35763,7 @@
       </c>
       <c r="AG179" s="32"/>
       <c r="AI179" s="32" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="AJ179" s="32" t="str">
         <f t="shared" si="200"/>
@@ -35847,7 +35865,7 @@
       </c>
       <c r="AG180" s="32"/>
       <c r="AI180" s="32" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="AJ180" s="32" t="str">
         <f t="shared" si="200"/>
@@ -35949,7 +35967,7 @@
       </c>
       <c r="AG181" s="32"/>
       <c r="AI181" s="32" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="AJ181" s="32" t="str">
         <f t="shared" si="200"/>
@@ -36051,7 +36069,7 @@
       </c>
       <c r="AG182" s="32"/>
       <c r="AI182" s="32" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="AJ182" s="32" t="str">
         <f t="shared" si="200"/>
@@ -36153,7 +36171,7 @@
       </c>
       <c r="AG183" s="32"/>
       <c r="AI183" s="32" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="AJ183" s="32" t="str">
         <f t="shared" si="200"/>
@@ -36255,7 +36273,7 @@
       </c>
       <c r="AG184" s="32"/>
       <c r="AI184" s="32" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="AJ184" s="32" t="str">
         <f t="shared" si="200"/>
@@ -36344,7 +36362,7 @@
       </c>
       <c r="AG185" s="32"/>
       <c r="AI185" s="32" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="AJ185" s="32" t="str">
         <f t="shared" si="200"/>
@@ -36433,7 +36451,7 @@
       </c>
       <c r="AG186" s="32"/>
       <c r="AI186" s="32" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="AJ186" s="32" t="str">
         <f t="shared" si="200"/>
@@ -41882,7 +41900,7 @@
         <v>914</v>
       </c>
       <c r="D5" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -41893,7 +41911,7 @@
         <v>916</v>
       </c>
       <c r="D6" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -41912,7 +41930,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -41926,7 +41944,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -41934,7 +41952,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="D10">
         <v>9</v>
@@ -41942,7 +41960,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -41950,34 +41968,34 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="D12" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="D13" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="D14" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="D15" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
     </row>
   </sheetData>
@@ -42020,19 +42038,19 @@
         <v>907</v>
       </c>
       <c r="C3" t="s">
+        <v>1233</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1237</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1234</v>
+      </c>
+      <c r="G3" t="s">
         <v>1235</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1239</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1240</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1236</v>
-      </c>
-      <c r="G3" t="s">
-        <v>1237</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -42040,10 +42058,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="C4" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -42060,10 +42078,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="C5" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -42083,10 +42101,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="C6" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -42100,10 +42118,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="C7" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -42117,10 +42135,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="C8" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -42134,10 +42152,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="C9" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -42151,10 +42169,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="C10" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -42171,10 +42189,10 @@
         <v>7</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="C11" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -42191,10 +42209,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="C12" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="D12">
         <v>4</v>

</xml_diff>

<commit_message>
Notes for field mods
</commit_message>
<xml_diff>
--- a/syscon_usb/DACS_V1_0_ISE/tools/dacs.ucf.xlsx
+++ b/syscon_usb/DACS_V1_0_ISE/tools/dacs.ucf.xlsx
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Board!$J$148:$J$162</definedName>
   </definedNames>
-  <calcPr calcId="125725" calcMode="manual"/>
+  <calcPr calcId="125725" calcMode="manual" calcCompleted="0"/>
 </workbook>
 </file>
 
@@ -59,8 +59,66 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Norton Allen</author>
+  </authors>
+  <commentList>
+    <comment ref="AI134" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Norton Allen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+dccc is using dig_IO&lt;101&gt; to addres DIO_5Sp.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AI233" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Norton Allen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Ports 13-24 are all input, so I am going to skip them in dccc. Dccc will think this port is port 13. It will also think this line is dig_IO&lt;101&gt;.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3711" uniqueCount="1282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3711" uniqueCount="1283">
   <si>
     <t>IOSTANDARD</t>
   </si>
@@ -3906,13 +3964,16 @@
   </si>
   <si>
     <t>InverterArm_Off</t>
+  </si>
+  <si>
+    <t>DIO_5Sp/BAT Purge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="22">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4071,6 +4132,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="37">
@@ -10942,10 +11016,10 @@
   <dimension ref="A1:U137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="O51" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="P18" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S57" sqref="S57"/>
+      <selection pane="bottomRight" activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18582,10 +18656,10 @@
   <dimension ref="A1:AL272"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AA128" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="AA123" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="F2" sqref="F1:F1048576"/>
       <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
-      <selection pane="bottomRight" activeCell="AI145" sqref="AI145"/>
+      <selection pane="bottomRight" activeCell="AI134" sqref="AI134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40125,7 +40199,7 @@
         <v>314</v>
       </c>
       <c r="AI233" s="32" t="s">
-        <v>1045</v>
+        <v>1282</v>
       </c>
       <c r="AJ233" s="32" t="str">
         <f t="shared" si="229"/>
@@ -41609,6 +41683,7 @@
   <ignoredErrors>
     <ignoredError sqref="U34:U35 U37:U38 U40:U45 U46 U49 U52 U54 U56 U58 U60 U62 U64 U66 U68 U70 U72 U74 U76 U78 U80 U82 U84 U86 U88 U90 U92 U94" formula="1"/>
   </ignoredErrors>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>